<commit_message>
Small tweeks to the formating
</commit_message>
<xml_diff>
--- a/Bracket.xlsx
+++ b/Bracket.xlsx
@@ -12,9 +12,12 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="20460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Bracket" sheetId="1" r:id="rId1"/>
+    <sheet name="Competitors" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Competitors!$A:$D</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -212,9 +215,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="18"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial Unicode MS"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="3">
@@ -470,7 +473,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -611,11 +614,14 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1143,7 +1149,7 @@
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="90"/>
+      <c r="J3" s="89"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="10"/>
@@ -2800,6 +2806,11 @@
   <ignoredErrors>
     <ignoredError sqref="B59" emptyCellReference="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2820,51 +2831,53 @@
       <c r="A1" s="88" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="88">
-        <f>Sheet1!Q1</f>
+      <c r="B1" s="90">
+        <f>Bracket!Q1</f>
         <v>0</v>
       </c>
       <c r="C1" s="88"/>
       <c r="D1" s="88"/>
     </row>
-    <row r="2" spans="1:4" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="89">
-        <f>Sheet1!B3</f>
-        <v>0</v>
-      </c>
-      <c r="B2" s="88">
-        <f>Sheet1!F3</f>
-        <v>0</v>
-      </c>
-      <c r="C2" s="88">
-        <f>Sheet1!J3</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="88">
-        <f>Sheet1!N3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="88">
-        <f>Sheet1!B4</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="88">
-        <f>Sheet1!F4</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="88">
-        <f>Sheet1!J4</f>
-        <v>0</v>
-      </c>
-      <c r="D3" s="88">
-        <f>Sheet1!N4</f>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="91">
+        <f>Bracket!B3</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="91">
+        <f>Bracket!F3</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="91">
+        <f>Bracket!J3</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="91">
+        <f>Bracket!N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="91">
+        <f>Bracket!B4</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="91">
+        <f>Bracket!F4</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="91">
+        <f>Bracket!J4</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="91">
+        <f>Bracket!N4</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetProtection password="CFAF" sheet="1" objects="1" scenarios="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removing names and adding just group instead of weight group.
</commit_message>
<xml_diff>
--- a/Bracket.xlsx
+++ b/Bracket.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="34">
   <si>
     <t></t>
   </si>
@@ -36,9 +36,6 @@
     <t></t>
   </si>
   <si>
-    <t>Weight Group:</t>
-  </si>
-  <si>
     <t>Wrestler #1</t>
   </si>
   <si>
@@ -129,22 +126,10 @@
     <t>Bracket/Mat #:</t>
   </si>
   <si>
-    <t>Bracket/Mat#</t>
-  </si>
-  <si>
-    <t>Johnathan Thomas McBrides</t>
-  </si>
-  <si>
-    <t>WR</t>
-  </si>
-  <si>
-    <t>Brendan James McBride</t>
-  </si>
-  <si>
-    <t>Some Body Else with a long</t>
-  </si>
-  <si>
-    <t>Another long long name</t>
+    <t>Group:</t>
+  </si>
+  <si>
+    <t>Group/Mat#</t>
   </si>
 </sst>
 </file>
@@ -525,7 +510,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -616,69 +601,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -688,8 +610,85 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="111">
@@ -1140,7 +1139,7 @@
   <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="N4" sqref="N4:Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1153,7 +1152,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="8" customFormat="1" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -1168,42 +1167,40 @@
       </c>
       <c r="H1" s="40"/>
       <c r="I1" s="37" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="J1" s="41"/>
       <c r="K1" s="39"/>
       <c r="L1" s="48"/>
       <c r="M1" s="40"/>
       <c r="N1" s="37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O1" s="39"/>
       <c r="P1" s="49"/>
-      <c r="Q1" s="50">
-        <v>6</v>
-      </c>
+      <c r="Q1" s="50"/>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="43"/>
       <c r="F2" s="44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="45"/>
       <c r="H2" s="45"/>
       <c r="I2" s="46"/>
       <c r="J2" s="47" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
       <c r="M2" s="43"/>
       <c r="N2" s="42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O2" s="16"/>
       <c r="P2" s="16"/>
@@ -1211,78 +1208,62 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="65" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="55"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56"/>
-      <c r="N3" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="55"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="56"/>
+        <v>28</v>
+      </c>
+      <c r="B3" s="88"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="94"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="93"/>
+      <c r="P3" s="93"/>
+      <c r="Q3" s="94"/>
     </row>
     <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="79" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="59"/>
+        <v>29</v>
+      </c>
+      <c r="B4" s="89"/>
+      <c r="C4" s="95"/>
+      <c r="D4" s="95"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="97"/>
+      <c r="L4" s="97"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="95"/>
+      <c r="P4" s="95"/>
+      <c r="Q4" s="96"/>
     </row>
     <row r="5" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="71"/>
+      <c r="B6" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="69"/>
+      <c r="D6" s="70"/>
     </row>
     <row r="7" spans="1:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="75" t="s">
-        <v>6</v>
+      <c r="B7" s="71" t="s">
+        <v>5</v>
       </c>
       <c r="C7" s="61"/>
-      <c r="D7" s="62"/>
+      <c r="D7" s="60"/>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1291,7 +1272,7 @@
       <c r="J7" s="31"/>
       <c r="K7" s="3"/>
       <c r="L7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1300,11 +1281,11 @@
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="83" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
+      <c r="B8" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="65"/>
+      <c r="D8" s="66"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1320,218 +1301,218 @@
       <c r="Q8" s="6"/>
     </row>
     <row r="9" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="60" t="s">
-        <v>3</v>
+      <c r="B9" s="59" t="s">
+        <v>2</v>
       </c>
       <c r="C9" s="61"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="60" t="s">
+      <c r="D9" s="60"/>
+      <c r="E9" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="61"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="60" t="s">
+      <c r="I9" s="61"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="61"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="60" t="s">
+      <c r="L9" s="61"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="L9" s="61"/>
-      <c r="M9" s="62"/>
-      <c r="N9" s="60" t="s">
+      <c r="O9" s="60"/>
+      <c r="P9" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="62"/>
-      <c r="P9" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="62"/>
+      <c r="Q9" s="60"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="54" t="str">
+      <c r="B10" s="78" t="str">
         <f>IF(B3="","",B3)</f>
-        <v>Johnathan Thomas McBrides</v>
-      </c>
-      <c r="C10" s="55"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="55"/>
+        <v/>
+      </c>
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="75"/>
       <c r="J10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="54"/>
-      <c r="L10" s="55"/>
+      <c r="K10" s="78"/>
+      <c r="L10" s="75"/>
       <c r="M10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="54"/>
-      <c r="O10" s="56"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="56"/>
+      <c r="N10" s="78"/>
+      <c r="O10" s="76"/>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="76"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="54" t="str">
+      <c r="B11" s="78" t="str">
         <f>IF(B4="","",B4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="55"/>
+        <v/>
+      </c>
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="75"/>
       <c r="J11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" s="54"/>
-      <c r="L11" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K11" s="78"/>
+      <c r="L11" s="75"/>
       <c r="M11" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N11" s="54"/>
-      <c r="O11" s="56"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N11" s="78"/>
+      <c r="O11" s="76"/>
+      <c r="P11" s="78"/>
+      <c r="Q11" s="76"/>
     </row>
     <row r="12" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="58"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="65"/>
       <c r="J12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K12" s="57"/>
-      <c r="L12" s="58"/>
+      <c r="K12" s="77"/>
+      <c r="L12" s="65"/>
       <c r="M12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N12" s="57"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="57"/>
-      <c r="Q12" s="59"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="66"/>
     </row>
     <row r="13" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="60" t="s">
-        <v>8</v>
+      <c r="B13" s="59" t="s">
+        <v>7</v>
       </c>
       <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="60" t="s">
+      <c r="D13" s="60"/>
+      <c r="E13" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="61"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="60" t="s">
+      <c r="I13" s="61"/>
+      <c r="J13" s="60"/>
+      <c r="K13" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="60" t="s">
+      <c r="L13" s="61"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L13" s="61"/>
-      <c r="M13" s="62"/>
-      <c r="N13" s="87" t="s">
+      <c r="O13" s="60"/>
+      <c r="P13" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="O13" s="62"/>
-      <c r="P13" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q13" s="62"/>
+      <c r="Q13" s="60"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B14" s="54" t="str">
+      <c r="B14" s="78" t="str">
         <f>IF(F3="","",F3)</f>
-        <v>Brendan James McBride</v>
-      </c>
-      <c r="C14" s="55"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="55"/>
+        <v/>
+      </c>
+      <c r="C14" s="75"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="75"/>
       <c r="J14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="54"/>
-      <c r="L14" s="55"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="75"/>
       <c r="M14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N14" s="66"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="56"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="76"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="76"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="54" t="str">
+      <c r="B15" s="78" t="str">
         <f>IF(F4="","",F4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="55"/>
+        <v/>
+      </c>
+      <c r="C15" s="75"/>
+      <c r="D15" s="76"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="78"/>
+      <c r="I15" s="75"/>
       <c r="J15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K15" s="54"/>
-      <c r="L15" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K15" s="78"/>
+      <c r="L15" s="75"/>
       <c r="M15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N15" s="54"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="54"/>
-      <c r="Q15" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N15" s="78"/>
+      <c r="O15" s="76"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="76"/>
     </row>
     <row r="16" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="59"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="58"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="66"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="65"/>
       <c r="J16" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="57"/>
-      <c r="L16" s="58"/>
+      <c r="K16" s="77"/>
+      <c r="L16" s="65"/>
       <c r="M16" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N16" s="57"/>
-      <c r="O16" s="59"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="59"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="77"/>
+      <c r="Q16" s="66"/>
     </row>
     <row r="17" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="75" t="s">
-        <v>6</v>
+      <c r="B18" s="71" t="s">
+        <v>5</v>
       </c>
       <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
+      <c r="D18" s="60"/>
       <c r="E18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1540,7 +1521,7 @@
       <c r="J18" s="31"/>
       <c r="K18" s="3"/>
       <c r="L18" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1549,11 +1530,11 @@
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="83" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="59"/>
+      <c r="B19" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="65"/>
+      <c r="D19" s="66"/>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1569,208 +1550,208 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="60" t="s">
-        <v>4</v>
+      <c r="B20" s="59" t="s">
+        <v>3</v>
       </c>
       <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="60" t="s">
+      <c r="D20" s="60"/>
+      <c r="E20" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="61"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="60" t="s">
+      <c r="I20" s="61"/>
+      <c r="J20" s="60"/>
+      <c r="K20" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="61"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="60" t="s">
+      <c r="L20" s="61"/>
+      <c r="M20" s="60"/>
+      <c r="N20" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="L20" s="61"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="60" t="s">
+      <c r="O20" s="60"/>
+      <c r="P20" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="O20" s="62"/>
-      <c r="P20" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q20" s="62"/>
+      <c r="Q20" s="60"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="54" t="str">
+      <c r="B21" s="78" t="str">
         <f>IF(J3="","",J3)</f>
-        <v>Some Body Else with a long</v>
-      </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="55"/>
+        <v/>
+      </c>
+      <c r="C21" s="75"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="78"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="78"/>
+      <c r="I21" s="75"/>
       <c r="J21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="55"/>
+      <c r="K21" s="78"/>
+      <c r="L21" s="75"/>
       <c r="M21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="54"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="54"/>
-      <c r="Q21" s="56"/>
+      <c r="N21" s="78"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="78"/>
+      <c r="Q21" s="76"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="54" t="str">
+      <c r="B22" s="78" t="str">
         <f>IF(J4="","",J4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="55"/>
+        <v/>
+      </c>
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="78"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="78"/>
+      <c r="I22" s="75"/>
       <c r="J22" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K22" s="78"/>
+      <c r="L22" s="75"/>
       <c r="M22" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N22" s="54"/>
-      <c r="O22" s="56"/>
-      <c r="P22" s="54"/>
-      <c r="Q22" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N22" s="78"/>
+      <c r="O22" s="76"/>
+      <c r="P22" s="78"/>
+      <c r="Q22" s="76"/>
     </row>
     <row r="23" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="58"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="66"/>
+      <c r="H23" s="77"/>
+      <c r="I23" s="65"/>
       <c r="J23" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K23" s="57"/>
-      <c r="L23" s="58"/>
+      <c r="K23" s="77"/>
+      <c r="L23" s="65"/>
       <c r="M23" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N23" s="57"/>
-      <c r="O23" s="59"/>
-      <c r="P23" s="57"/>
-      <c r="Q23" s="59"/>
+      <c r="N23" s="77"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="66"/>
     </row>
     <row r="24" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="60" t="s">
-        <v>5</v>
+      <c r="B24" s="59" t="s">
+        <v>4</v>
       </c>
       <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="60" t="s">
+      <c r="D24" s="60"/>
+      <c r="E24" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="61"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="61"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="60" t="s">
+      <c r="I24" s="61"/>
+      <c r="J24" s="60"/>
+      <c r="K24" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="61"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="60" t="s">
+      <c r="L24" s="61"/>
+      <c r="M24" s="60"/>
+      <c r="N24" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L24" s="61"/>
-      <c r="M24" s="62"/>
-      <c r="N24" s="87" t="s">
+      <c r="O24" s="60"/>
+      <c r="P24" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="O24" s="62"/>
-      <c r="P24" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q24" s="62"/>
+      <c r="Q24" s="60"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="54" t="str">
+      <c r="B25" s="78" t="str">
         <f>IF(N3="","",N3)</f>
-        <v>Another long long name</v>
-      </c>
-      <c r="C25" s="55"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="55"/>
+        <v/>
+      </c>
+      <c r="C25" s="75"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="76"/>
+      <c r="H25" s="78"/>
+      <c r="I25" s="75"/>
       <c r="J25" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="55"/>
+      <c r="K25" s="78"/>
+      <c r="L25" s="75"/>
       <c r="M25" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N25" s="66"/>
-      <c r="O25" s="56"/>
-      <c r="P25" s="54"/>
-      <c r="Q25" s="56"/>
+      <c r="N25" s="85"/>
+      <c r="O25" s="76"/>
+      <c r="P25" s="78"/>
+      <c r="Q25" s="76"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="54" t="str">
+      <c r="B26" s="78" t="str">
         <f>IF(N4="","",N4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="54"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="55"/>
+        <v/>
+      </c>
+      <c r="C26" s="75"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="78"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="78"/>
+      <c r="I26" s="75"/>
       <c r="J26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K26" s="54"/>
-      <c r="L26" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K26" s="78"/>
+      <c r="L26" s="75"/>
       <c r="M26" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N26" s="54"/>
-      <c r="O26" s="56"/>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N26" s="78"/>
+      <c r="O26" s="76"/>
+      <c r="P26" s="78"/>
+      <c r="Q26" s="76"/>
     </row>
     <row r="27" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="58"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="77"/>
+      <c r="I27" s="65"/>
       <c r="J27" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K27" s="57"/>
-      <c r="L27" s="58"/>
+      <c r="K27" s="77"/>
+      <c r="L27" s="65"/>
       <c r="M27" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="57"/>
-      <c r="O27" s="59"/>
-      <c r="P27" s="57"/>
-      <c r="Q27" s="59"/>
+      <c r="N27" s="77"/>
+      <c r="O27" s="66"/>
+      <c r="P27" s="77"/>
+      <c r="Q27" s="66"/>
     </row>
     <row r="28" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
@@ -1808,20 +1789,20 @@
     </row>
     <row r="30" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="82" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="71"/>
+      <c r="B31" s="68" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="69"/>
+      <c r="D31" s="70"/>
     </row>
     <row r="32" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="84" t="s">
-        <v>18</v>
+      <c r="B32" s="67" t="s">
+        <v>17</v>
       </c>
       <c r="C32" s="61"/>
-      <c r="D32" s="62"/>
+      <c r="D32" s="60"/>
       <c r="E32" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -1830,7 +1811,7 @@
       <c r="J32" s="33"/>
       <c r="K32" s="17"/>
       <c r="L32" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
@@ -1839,11 +1820,11 @@
       <c r="Q32" s="17"/>
     </row>
     <row r="33" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="85" t="s">
-        <v>25</v>
-      </c>
-      <c r="C33" s="58"/>
-      <c r="D33" s="59"/>
+      <c r="B33" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="65"/>
+      <c r="D33" s="66"/>
       <c r="E33" s="20"/>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
@@ -1859,217 +1840,217 @@
       <c r="Q33" s="22"/>
     </row>
     <row r="34" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="86" t="s">
-        <v>3</v>
+      <c r="B34" s="63" t="s">
+        <v>2</v>
       </c>
       <c r="C34" s="61"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="86" t="s">
+      <c r="D34" s="60"/>
+      <c r="E34" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="61"/>
+      <c r="G34" s="60"/>
+      <c r="H34" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="61"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="86" t="s">
+      <c r="I34" s="61"/>
+      <c r="J34" s="60"/>
+      <c r="K34" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I34" s="61"/>
-      <c r="J34" s="62"/>
-      <c r="K34" s="86" t="s">
+      <c r="L34" s="61"/>
+      <c r="M34" s="60"/>
+      <c r="N34" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="L34" s="61"/>
-      <c r="M34" s="62"/>
-      <c r="N34" s="86" t="s">
+      <c r="O34" s="60"/>
+      <c r="P34" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="O34" s="62"/>
-      <c r="P34" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q34" s="62"/>
+      <c r="Q34" s="60"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B35" s="67" t="str">
+      <c r="B35" s="86" t="str">
         <f>IF(B3="","",B3)</f>
-        <v>Johnathan Thomas McBrides</v>
-      </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="55"/>
-      <c r="G35" s="56"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="55"/>
+        <v/>
+      </c>
+      <c r="C35" s="75"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="86"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="86"/>
+      <c r="I35" s="75"/>
       <c r="J35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="67"/>
-      <c r="L35" s="55"/>
+      <c r="K35" s="86"/>
+      <c r="L35" s="75"/>
       <c r="M35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N35" s="67"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="67"/>
-      <c r="Q35" s="56"/>
+      <c r="N35" s="86"/>
+      <c r="O35" s="76"/>
+      <c r="P35" s="86"/>
+      <c r="Q35" s="76"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="67" t="str">
+      <c r="B36" s="86" t="str">
         <f>IF(B4="","",B4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C36" s="55"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="55"/>
+        <v/>
+      </c>
+      <c r="C36" s="75"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="78"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="78"/>
+      <c r="I36" s="75"/>
       <c r="J36" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="K36" s="54"/>
-      <c r="L36" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K36" s="78"/>
+      <c r="L36" s="75"/>
       <c r="M36" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" s="54"/>
-      <c r="O36" s="56"/>
-      <c r="P36" s="54"/>
-      <c r="Q36" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N36" s="78"/>
+      <c r="O36" s="76"/>
+      <c r="P36" s="78"/>
+      <c r="Q36" s="76"/>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="20"/>
       <c r="C37" s="21"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="57"/>
-      <c r="I37" s="58"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="65"/>
       <c r="J37" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="K37" s="57"/>
-      <c r="L37" s="58"/>
+      <c r="K37" s="77"/>
+      <c r="L37" s="65"/>
       <c r="M37" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="N37" s="57"/>
-      <c r="O37" s="59"/>
-      <c r="P37" s="57"/>
-      <c r="Q37" s="59"/>
+      <c r="N37" s="77"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="77"/>
+      <c r="Q37" s="66"/>
     </row>
     <row r="38" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="86" t="s">
-        <v>4</v>
+      <c r="B38" s="63" t="s">
+        <v>3</v>
       </c>
       <c r="C38" s="61"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="86" t="s">
+      <c r="D38" s="60"/>
+      <c r="E38" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="61"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="F38" s="61"/>
-      <c r="G38" s="62"/>
-      <c r="H38" s="86" t="s">
+      <c r="I38" s="61"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I38" s="61"/>
-      <c r="J38" s="62"/>
-      <c r="K38" s="86" t="s">
+      <c r="L38" s="61"/>
+      <c r="M38" s="60"/>
+      <c r="N38" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="L38" s="61"/>
-      <c r="M38" s="62"/>
-      <c r="N38" s="88" t="s">
+      <c r="O38" s="60"/>
+      <c r="P38" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="O38" s="62"/>
-      <c r="P38" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q38" s="62"/>
+      <c r="Q38" s="60"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B39" s="67" t="str">
+      <c r="B39" s="86" t="str">
         <f>IF(J3="","",J3)</f>
-        <v>Some Body Else with a long</v>
-      </c>
-      <c r="C39" s="55"/>
-      <c r="D39" s="56"/>
-      <c r="E39" s="67"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="56"/>
-      <c r="H39" s="67"/>
-      <c r="I39" s="55"/>
+        <v/>
+      </c>
+      <c r="C39" s="75"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="86"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="86"/>
+      <c r="I39" s="75"/>
       <c r="J39" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K39" s="67"/>
-      <c r="L39" s="55"/>
+      <c r="K39" s="86"/>
+      <c r="L39" s="75"/>
       <c r="M39" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N39" s="68"/>
-      <c r="O39" s="56"/>
-      <c r="P39" s="67"/>
-      <c r="Q39" s="56"/>
+      <c r="N39" s="87"/>
+      <c r="O39" s="76"/>
+      <c r="P39" s="86"/>
+      <c r="Q39" s="76"/>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B40" s="67" t="str">
+      <c r="B40" s="86" t="str">
         <f>IF(J4="","",J4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C40" s="55"/>
-      <c r="D40" s="56"/>
-      <c r="E40" s="54"/>
-      <c r="F40" s="55"/>
-      <c r="G40" s="56"/>
-      <c r="H40" s="54"/>
-      <c r="I40" s="55"/>
+        <v/>
+      </c>
+      <c r="C40" s="75"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="78"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="78"/>
+      <c r="I40" s="75"/>
       <c r="J40" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="K40" s="54"/>
-      <c r="L40" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K40" s="78"/>
+      <c r="L40" s="75"/>
       <c r="M40" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N40" s="54"/>
-      <c r="O40" s="56"/>
-      <c r="P40" s="54"/>
-      <c r="Q40" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N40" s="78"/>
+      <c r="O40" s="76"/>
+      <c r="P40" s="78"/>
+      <c r="Q40" s="76"/>
     </row>
     <row r="41" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="20"/>
       <c r="C41" s="21"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="57"/>
-      <c r="I41" s="58"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="65"/>
       <c r="J41" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="K41" s="57"/>
-      <c r="L41" s="58"/>
+      <c r="K41" s="77"/>
+      <c r="L41" s="65"/>
       <c r="M41" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="N41" s="57"/>
-      <c r="O41" s="59"/>
-      <c r="P41" s="57"/>
-      <c r="Q41" s="59"/>
+      <c r="N41" s="77"/>
+      <c r="O41" s="66"/>
+      <c r="P41" s="77"/>
+      <c r="Q41" s="66"/>
     </row>
     <row r="42" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="84" t="s">
-        <v>18</v>
+      <c r="B42" s="67" t="s">
+        <v>17</v>
       </c>
       <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
+      <c r="D42" s="60"/>
       <c r="E42" s="25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F42" s="29"/>
       <c r="G42" s="29"/>
@@ -2078,7 +2059,7 @@
       <c r="J42" s="35"/>
       <c r="K42" s="26"/>
       <c r="L42" s="25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M42" s="29"/>
       <c r="N42" s="29"/>
@@ -2087,11 +2068,11 @@
       <c r="Q42" s="26"/>
     </row>
     <row r="43" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="85" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
+      <c r="B43" s="64" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="65"/>
+      <c r="D43" s="66"/>
       <c r="E43" s="20"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -2107,208 +2088,208 @@
       <c r="Q43" s="22"/>
     </row>
     <row r="44" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="86" t="s">
-        <v>8</v>
+      <c r="B44" s="63" t="s">
+        <v>7</v>
       </c>
       <c r="C44" s="61"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="86" t="s">
+      <c r="D44" s="60"/>
+      <c r="E44" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="61"/>
+      <c r="G44" s="60"/>
+      <c r="H44" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="61"/>
-      <c r="G44" s="62"/>
-      <c r="H44" s="86" t="s">
+      <c r="I44" s="61"/>
+      <c r="J44" s="60"/>
+      <c r="K44" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="61"/>
-      <c r="J44" s="62"/>
-      <c r="K44" s="86" t="s">
+      <c r="L44" s="61"/>
+      <c r="M44" s="60"/>
+      <c r="N44" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="L44" s="61"/>
-      <c r="M44" s="62"/>
-      <c r="N44" s="86" t="s">
+      <c r="O44" s="60"/>
+      <c r="P44" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="O44" s="62"/>
-      <c r="P44" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q44" s="62"/>
+      <c r="Q44" s="60"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B45" s="67" t="str">
+      <c r="B45" s="86" t="str">
         <f>IF(F3="","",F3)</f>
-        <v>Brendan James McBride</v>
-      </c>
-      <c r="C45" s="55"/>
-      <c r="D45" s="56"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="56"/>
-      <c r="H45" s="67"/>
-      <c r="I45" s="55"/>
+        <v/>
+      </c>
+      <c r="C45" s="75"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="86"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="75"/>
       <c r="J45" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K45" s="67"/>
-      <c r="L45" s="55"/>
+      <c r="K45" s="86"/>
+      <c r="L45" s="75"/>
       <c r="M45" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N45" s="67"/>
-      <c r="O45" s="56"/>
-      <c r="P45" s="67"/>
-      <c r="Q45" s="56"/>
+      <c r="N45" s="86"/>
+      <c r="O45" s="76"/>
+      <c r="P45" s="86"/>
+      <c r="Q45" s="76"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B46" s="67" t="str">
+      <c r="B46" s="86" t="str">
         <f>IF(F4="","",F4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="56"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="55"/>
+        <v/>
+      </c>
+      <c r="C46" s="75"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="78"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="75"/>
       <c r="J46" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" s="54"/>
-      <c r="L46" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K46" s="78"/>
+      <c r="L46" s="75"/>
       <c r="M46" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N46" s="54"/>
-      <c r="O46" s="56"/>
-      <c r="P46" s="54"/>
-      <c r="Q46" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N46" s="78"/>
+      <c r="O46" s="76"/>
+      <c r="P46" s="78"/>
+      <c r="Q46" s="76"/>
     </row>
     <row r="47" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="20"/>
       <c r="C47" s="21"/>
       <c r="D47" s="22"/>
-      <c r="E47" s="57"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="59"/>
-      <c r="H47" s="57"/>
-      <c r="I47" s="58"/>
+      <c r="E47" s="77"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="66"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="65"/>
       <c r="J47" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="K47" s="57"/>
-      <c r="L47" s="58"/>
+      <c r="K47" s="77"/>
+      <c r="L47" s="65"/>
       <c r="M47" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="N47" s="57"/>
-      <c r="O47" s="59"/>
-      <c r="P47" s="57"/>
-      <c r="Q47" s="59"/>
+      <c r="N47" s="77"/>
+      <c r="O47" s="66"/>
+      <c r="P47" s="77"/>
+      <c r="Q47" s="66"/>
     </row>
     <row r="48" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="86" t="s">
-        <v>5</v>
+      <c r="B48" s="63" t="s">
+        <v>4</v>
       </c>
       <c r="C48" s="61"/>
-      <c r="D48" s="62"/>
-      <c r="E48" s="86" t="s">
+      <c r="D48" s="60"/>
+      <c r="E48" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="61"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="61"/>
-      <c r="G48" s="62"/>
-      <c r="H48" s="86" t="s">
+      <c r="I48" s="61"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="I48" s="61"/>
-      <c r="J48" s="62"/>
-      <c r="K48" s="86" t="s">
+      <c r="L48" s="61"/>
+      <c r="M48" s="60"/>
+      <c r="N48" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="L48" s="61"/>
-      <c r="M48" s="62"/>
-      <c r="N48" s="88" t="s">
+      <c r="O48" s="60"/>
+      <c r="P48" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="O48" s="62"/>
-      <c r="P48" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q48" s="62"/>
+      <c r="Q48" s="60"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B49" s="67" t="str">
+      <c r="B49" s="86" t="str">
         <f>IF(N3="","",N3)</f>
-        <v>Another long long name</v>
-      </c>
-      <c r="C49" s="55"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="67"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="56"/>
-      <c r="H49" s="67"/>
-      <c r="I49" s="55"/>
+        <v/>
+      </c>
+      <c r="C49" s="75"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="86"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="86"/>
+      <c r="I49" s="75"/>
       <c r="J49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K49" s="67"/>
-      <c r="L49" s="55"/>
+      <c r="K49" s="86"/>
+      <c r="L49" s="75"/>
       <c r="M49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N49" s="68"/>
-      <c r="O49" s="56"/>
-      <c r="P49" s="67"/>
-      <c r="Q49" s="56"/>
+      <c r="N49" s="87"/>
+      <c r="O49" s="76"/>
+      <c r="P49" s="86"/>
+      <c r="Q49" s="76"/>
     </row>
     <row r="50" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B50" s="67" t="str">
+      <c r="B50" s="86" t="str">
         <f>IF(N4="","",N4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C50" s="55"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="56"/>
-      <c r="H50" s="54"/>
-      <c r="I50" s="55"/>
+        <v/>
+      </c>
+      <c r="C50" s="75"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="78"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="78"/>
+      <c r="I50" s="75"/>
       <c r="J50" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="K50" s="54"/>
-      <c r="L50" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K50" s="78"/>
+      <c r="L50" s="75"/>
       <c r="M50" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="N50" s="54"/>
-      <c r="O50" s="56"/>
-      <c r="P50" s="54"/>
-      <c r="Q50" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N50" s="78"/>
+      <c r="O50" s="76"/>
+      <c r="P50" s="78"/>
+      <c r="Q50" s="76"/>
     </row>
     <row r="51" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="20"/>
       <c r="C51" s="21"/>
       <c r="D51" s="22"/>
-      <c r="E51" s="57"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="59"/>
-      <c r="H51" s="57"/>
-      <c r="I51" s="58"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="65"/>
+      <c r="G51" s="66"/>
+      <c r="H51" s="77"/>
+      <c r="I51" s="65"/>
       <c r="J51" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="K51" s="57"/>
-      <c r="L51" s="58"/>
+      <c r="K51" s="77"/>
+      <c r="L51" s="65"/>
       <c r="M51" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="N51" s="57"/>
-      <c r="O51" s="59"/>
-      <c r="P51" s="57"/>
-      <c r="Q51" s="59"/>
+      <c r="N51" s="77"/>
+      <c r="O51" s="66"/>
+      <c r="P51" s="77"/>
+      <c r="Q51" s="66"/>
     </row>
     <row r="52" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C52"/>
@@ -2320,20 +2301,20 @@
     </row>
     <row r="54" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="82" t="s">
-        <v>19</v>
-      </c>
-      <c r="C55" s="70"/>
-      <c r="D55" s="71"/>
+      <c r="B55" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="69"/>
+      <c r="D55" s="70"/>
     </row>
     <row r="56" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="75" t="s">
-        <v>19</v>
+      <c r="B56" s="71" t="s">
+        <v>18</v>
       </c>
       <c r="C56" s="61"/>
-      <c r="D56" s="62"/>
+      <c r="D56" s="60"/>
       <c r="E56" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -2342,7 +2323,7 @@
       <c r="J56" s="31"/>
       <c r="K56" s="3"/>
       <c r="L56" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -2351,11 +2332,11 @@
       <c r="Q56" s="3"/>
     </row>
     <row r="57" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="83" t="s">
-        <v>27</v>
-      </c>
-      <c r="C57" s="58"/>
-      <c r="D57" s="59"/>
+      <c r="B57" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="65"/>
+      <c r="D57" s="66"/>
       <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -2371,218 +2352,218 @@
       <c r="Q57" s="6"/>
     </row>
     <row r="58" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="60" t="s">
-        <v>3</v>
+      <c r="B58" s="59" t="s">
+        <v>2</v>
       </c>
       <c r="C58" s="61"/>
-      <c r="D58" s="62"/>
+      <c r="D58" s="60"/>
       <c r="E58" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="7"/>
       <c r="H58" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I58" s="2"/>
       <c r="J58" s="14"/>
       <c r="K58" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L58" s="2"/>
       <c r="M58" s="14"/>
       <c r="N58" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O58" s="3"/>
       <c r="P58" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q58" s="3"/>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B59" s="54" t="str">
+      <c r="B59" s="78" t="str">
         <f>IF(B3="","",B3)</f>
-        <v>Johnathan Thomas McBrides</v>
-      </c>
-      <c r="C59" s="55"/>
-      <c r="D59" s="56"/>
-      <c r="E59" s="54"/>
-      <c r="F59" s="55"/>
-      <c r="G59" s="56"/>
-      <c r="H59" s="54"/>
-      <c r="I59" s="55"/>
+        <v/>
+      </c>
+      <c r="C59" s="75"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="78"/>
+      <c r="F59" s="75"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="78"/>
+      <c r="I59" s="75"/>
       <c r="J59" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K59" s="54"/>
-      <c r="L59" s="55"/>
+      <c r="K59" s="78"/>
+      <c r="L59" s="75"/>
       <c r="M59" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N59" s="54"/>
-      <c r="O59" s="56"/>
-      <c r="P59" s="54"/>
-      <c r="Q59" s="56"/>
+      <c r="N59" s="78"/>
+      <c r="O59" s="76"/>
+      <c r="P59" s="78"/>
+      <c r="Q59" s="76"/>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B60" s="54" t="str">
+      <c r="B60" s="78" t="str">
         <f>IF(B4="","",B4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C60" s="55"/>
-      <c r="D60" s="56"/>
-      <c r="E60" s="54"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="56"/>
-      <c r="H60" s="54"/>
-      <c r="I60" s="55"/>
+        <v/>
+      </c>
+      <c r="C60" s="75"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="78"/>
+      <c r="F60" s="75"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="78"/>
+      <c r="I60" s="75"/>
       <c r="J60" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K60" s="54"/>
-      <c r="L60" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K60" s="78"/>
+      <c r="L60" s="75"/>
       <c r="M60" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N60" s="54"/>
-      <c r="O60" s="56"/>
-      <c r="P60" s="54"/>
-      <c r="Q60" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N60" s="78"/>
+      <c r="O60" s="76"/>
+      <c r="P60" s="78"/>
+      <c r="Q60" s="76"/>
     </row>
     <row r="61" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="57"/>
-      <c r="F61" s="58"/>
-      <c r="G61" s="59"/>
-      <c r="H61" s="57"/>
-      <c r="I61" s="58"/>
+      <c r="E61" s="77"/>
+      <c r="F61" s="65"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="77"/>
+      <c r="I61" s="65"/>
       <c r="J61" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K61" s="57"/>
-      <c r="L61" s="58"/>
+      <c r="K61" s="77"/>
+      <c r="L61" s="65"/>
       <c r="M61" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N61" s="57"/>
-      <c r="O61" s="59"/>
-      <c r="P61" s="57"/>
-      <c r="Q61" s="59"/>
+      <c r="N61" s="77"/>
+      <c r="O61" s="66"/>
+      <c r="P61" s="77"/>
+      <c r="Q61" s="66"/>
     </row>
     <row r="62" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="60" t="s">
-        <v>5</v>
+      <c r="B62" s="59" t="s">
+        <v>4</v>
       </c>
       <c r="C62" s="61"/>
-      <c r="D62" s="62"/>
+      <c r="D62" s="60"/>
       <c r="E62" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
       <c r="H62" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I62" s="2"/>
       <c r="J62" s="14"/>
       <c r="K62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L62" s="2"/>
       <c r="M62" s="14"/>
       <c r="N62" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O62" s="10"/>
       <c r="P62" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q62" s="3"/>
     </row>
     <row r="63" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B63" s="54" t="str">
+      <c r="B63" s="78" t="str">
         <f>IF(N3="","",N3)</f>
-        <v>Another long long name</v>
-      </c>
-      <c r="C63" s="55"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="55"/>
+        <v/>
+      </c>
+      <c r="C63" s="75"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="78"/>
+      <c r="F63" s="75"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="78"/>
+      <c r="I63" s="75"/>
       <c r="J63" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K63" s="54"/>
-      <c r="L63" s="55"/>
+      <c r="K63" s="78"/>
+      <c r="L63" s="75"/>
       <c r="M63" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N63" s="66"/>
-      <c r="O63" s="56"/>
-      <c r="P63" s="54"/>
-      <c r="Q63" s="56"/>
+      <c r="N63" s="85"/>
+      <c r="O63" s="76"/>
+      <c r="P63" s="78"/>
+      <c r="Q63" s="76"/>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B64" s="54" t="str">
+      <c r="B64" s="78" t="str">
         <f>IF(N4="","",N4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C64" s="55"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="55"/>
+        <v/>
+      </c>
+      <c r="C64" s="75"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="78"/>
+      <c r="F64" s="75"/>
+      <c r="G64" s="76"/>
+      <c r="H64" s="78"/>
+      <c r="I64" s="75"/>
       <c r="J64" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K64" s="54"/>
-      <c r="L64" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K64" s="78"/>
+      <c r="L64" s="75"/>
       <c r="M64" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N64" s="54"/>
-      <c r="O64" s="56"/>
-      <c r="P64" s="54"/>
-      <c r="Q64" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N64" s="78"/>
+      <c r="O64" s="76"/>
+      <c r="P64" s="78"/>
+      <c r="Q64" s="76"/>
     </row>
     <row r="65" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
-      <c r="E65" s="57"/>
-      <c r="F65" s="58"/>
-      <c r="G65" s="59"/>
-      <c r="H65" s="57"/>
-      <c r="I65" s="58"/>
+      <c r="E65" s="77"/>
+      <c r="F65" s="65"/>
+      <c r="G65" s="66"/>
+      <c r="H65" s="77"/>
+      <c r="I65" s="65"/>
       <c r="J65" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K65" s="57"/>
-      <c r="L65" s="58"/>
+      <c r="K65" s="77"/>
+      <c r="L65" s="65"/>
       <c r="M65" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N65" s="57"/>
-      <c r="O65" s="59"/>
-      <c r="P65" s="57"/>
-      <c r="Q65" s="59"/>
+      <c r="N65" s="77"/>
+      <c r="O65" s="66"/>
+      <c r="P65" s="77"/>
+      <c r="Q65" s="66"/>
     </row>
     <row r="66" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="75" t="s">
-        <v>19</v>
+      <c r="B67" s="71" t="s">
+        <v>18</v>
       </c>
       <c r="C67" s="61"/>
-      <c r="D67" s="62"/>
+      <c r="D67" s="60"/>
       <c r="E67" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -2591,7 +2572,7 @@
       <c r="J67" s="31"/>
       <c r="K67" s="3"/>
       <c r="L67" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -2600,11 +2581,11 @@
       <c r="Q67" s="3"/>
     </row>
     <row r="68" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="83" t="s">
-        <v>28</v>
-      </c>
-      <c r="C68" s="58"/>
-      <c r="D68" s="59"/>
+      <c r="B68" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="65"/>
+      <c r="D68" s="66"/>
       <c r="E68" s="4"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
@@ -2620,450 +2601,298 @@
       <c r="Q68" s="6"/>
     </row>
     <row r="69" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="60" t="s">
-        <v>8</v>
+      <c r="B69" s="59" t="s">
+        <v>7</v>
       </c>
       <c r="C69" s="61"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="60" t="s">
+      <c r="D69" s="60"/>
+      <c r="E69" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F69" s="61"/>
+      <c r="G69" s="60"/>
+      <c r="H69" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F69" s="61"/>
-      <c r="G69" s="62"/>
-      <c r="H69" s="60" t="s">
+      <c r="I69" s="61"/>
+      <c r="J69" s="60"/>
+      <c r="K69" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I69" s="61"/>
-      <c r="J69" s="62"/>
-      <c r="K69" s="60" t="s">
+      <c r="L69" s="61"/>
+      <c r="M69" s="60"/>
+      <c r="N69" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="L69" s="61"/>
-      <c r="M69" s="62"/>
-      <c r="N69" s="60" t="s">
+      <c r="O69" s="60"/>
+      <c r="P69" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="O69" s="62"/>
-      <c r="P69" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q69" s="62"/>
+      <c r="Q69" s="60"/>
     </row>
     <row r="70" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B70" s="54" t="str">
+      <c r="B70" s="78" t="str">
         <f>IF(F3="","",F3)</f>
-        <v>Brendan James McBride</v>
-      </c>
-      <c r="C70" s="55"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="55"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="55"/>
+        <v/>
+      </c>
+      <c r="C70" s="75"/>
+      <c r="D70" s="76"/>
+      <c r="E70" s="78"/>
+      <c r="F70" s="75"/>
+      <c r="G70" s="76"/>
+      <c r="H70" s="78"/>
+      <c r="I70" s="75"/>
       <c r="J70" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K70" s="54"/>
-      <c r="L70" s="55"/>
+      <c r="K70" s="78"/>
+      <c r="L70" s="75"/>
       <c r="M70" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N70" s="54"/>
-      <c r="O70" s="56"/>
-      <c r="P70" s="54"/>
-      <c r="Q70" s="56"/>
+      <c r="N70" s="78"/>
+      <c r="O70" s="76"/>
+      <c r="P70" s="78"/>
+      <c r="Q70" s="76"/>
     </row>
     <row r="71" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B71" s="54" t="str">
+      <c r="B71" s="78" t="str">
         <f>IF(F4="","",F4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C71" s="55"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="55"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="54"/>
-      <c r="I71" s="55"/>
+        <v/>
+      </c>
+      <c r="C71" s="75"/>
+      <c r="D71" s="76"/>
+      <c r="E71" s="78"/>
+      <c r="F71" s="75"/>
+      <c r="G71" s="76"/>
+      <c r="H71" s="78"/>
+      <c r="I71" s="75"/>
       <c r="J71" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K71" s="54"/>
-      <c r="L71" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K71" s="78"/>
+      <c r="L71" s="75"/>
       <c r="M71" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N71" s="54"/>
-      <c r="O71" s="56"/>
-      <c r="P71" s="54"/>
-      <c r="Q71" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N71" s="78"/>
+      <c r="O71" s="76"/>
+      <c r="P71" s="78"/>
+      <c r="Q71" s="76"/>
     </row>
     <row r="72" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
-      <c r="E72" s="57"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="59"/>
-      <c r="H72" s="57"/>
-      <c r="I72" s="58"/>
+      <c r="E72" s="77"/>
+      <c r="F72" s="65"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="77"/>
+      <c r="I72" s="65"/>
       <c r="J72" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K72" s="57"/>
-      <c r="L72" s="58"/>
+      <c r="K72" s="77"/>
+      <c r="L72" s="65"/>
       <c r="M72" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N72" s="57"/>
-      <c r="O72" s="59"/>
-      <c r="P72" s="57"/>
-      <c r="Q72" s="59"/>
+      <c r="N72" s="77"/>
+      <c r="O72" s="66"/>
+      <c r="P72" s="77"/>
+      <c r="Q72" s="66"/>
     </row>
     <row r="73" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="60" t="s">
-        <v>4</v>
+      <c r="B73" s="59" t="s">
+        <v>3</v>
       </c>
       <c r="C73" s="61"/>
-      <c r="D73" s="62"/>
-      <c r="E73" s="60" t="s">
+      <c r="D73" s="60"/>
+      <c r="E73" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="61"/>
+      <c r="G73" s="60"/>
+      <c r="H73" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="F73" s="61"/>
-      <c r="G73" s="62"/>
-      <c r="H73" s="60" t="s">
+      <c r="I73" s="61"/>
+      <c r="J73" s="60"/>
+      <c r="K73" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I73" s="61"/>
-      <c r="J73" s="62"/>
-      <c r="K73" s="60" t="s">
+      <c r="L73" s="61"/>
+      <c r="M73" s="60"/>
+      <c r="N73" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="L73" s="61"/>
-      <c r="M73" s="62"/>
-      <c r="N73" s="87" t="s">
+      <c r="O73" s="60"/>
+      <c r="P73" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="O73" s="62"/>
-      <c r="P73" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q73" s="62"/>
+      <c r="Q73" s="60"/>
     </row>
     <row r="74" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B74" s="54" t="str">
+      <c r="B74" s="78" t="str">
         <f>IF(J3="","",J3)</f>
-        <v>Some Body Else with a long</v>
-      </c>
-      <c r="C74" s="55"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="54"/>
-      <c r="F74" s="55"/>
-      <c r="G74" s="56"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="55"/>
+        <v/>
+      </c>
+      <c r="C74" s="75"/>
+      <c r="D74" s="76"/>
+      <c r="E74" s="78"/>
+      <c r="F74" s="75"/>
+      <c r="G74" s="76"/>
+      <c r="H74" s="78"/>
+      <c r="I74" s="75"/>
       <c r="J74" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K74" s="54"/>
-      <c r="L74" s="55"/>
+      <c r="K74" s="78"/>
+      <c r="L74" s="75"/>
       <c r="M74" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N74" s="66"/>
-      <c r="O74" s="56"/>
-      <c r="P74" s="54"/>
-      <c r="Q74" s="56"/>
+      <c r="N74" s="85"/>
+      <c r="O74" s="76"/>
+      <c r="P74" s="78"/>
+      <c r="Q74" s="76"/>
     </row>
     <row r="75" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B75" s="54" t="str">
+      <c r="B75" s="78" t="str">
         <f>IF(J4="","",J4)</f>
-        <v>WR</v>
-      </c>
-      <c r="C75" s="55"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="55"/>
-      <c r="G75" s="56"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="55"/>
+        <v/>
+      </c>
+      <c r="C75" s="75"/>
+      <c r="D75" s="76"/>
+      <c r="E75" s="78"/>
+      <c r="F75" s="75"/>
+      <c r="G75" s="76"/>
+      <c r="H75" s="78"/>
+      <c r="I75" s="75"/>
       <c r="J75" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="K75" s="54"/>
-      <c r="L75" s="55"/>
+        <v>15</v>
+      </c>
+      <c r="K75" s="78"/>
+      <c r="L75" s="75"/>
       <c r="M75" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N75" s="54"/>
-      <c r="O75" s="56"/>
-      <c r="P75" s="54"/>
-      <c r="Q75" s="56"/>
+        <v>15</v>
+      </c>
+      <c r="N75" s="78"/>
+      <c r="O75" s="76"/>
+      <c r="P75" s="78"/>
+      <c r="Q75" s="76"/>
     </row>
     <row r="76" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
-      <c r="E76" s="57"/>
-      <c r="F76" s="58"/>
-      <c r="G76" s="59"/>
-      <c r="H76" s="57"/>
-      <c r="I76" s="58"/>
+      <c r="E76" s="77"/>
+      <c r="F76" s="65"/>
+      <c r="G76" s="66"/>
+      <c r="H76" s="77"/>
+      <c r="I76" s="65"/>
       <c r="J76" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K76" s="57"/>
-      <c r="L76" s="58"/>
+      <c r="K76" s="77"/>
+      <c r="L76" s="65"/>
       <c r="M76" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N76" s="57"/>
-      <c r="O76" s="59"/>
-      <c r="P76" s="57"/>
-      <c r="Q76" s="59"/>
+      <c r="N76" s="77"/>
+      <c r="O76" s="66"/>
+      <c r="P76" s="77"/>
+      <c r="Q76" s="66"/>
     </row>
     <row r="77" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="78" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="2:17" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="72" t="s">
+      <c r="B79" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="C79" s="80"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="80"/>
+      <c r="F79" s="80"/>
+      <c r="G79" s="80"/>
+      <c r="H79" s="80"/>
+      <c r="I79" s="80"/>
+      <c r="J79" s="80"/>
+      <c r="K79" s="80"/>
+      <c r="L79" s="80"/>
+      <c r="M79" s="80"/>
+      <c r="N79" s="80"/>
+      <c r="O79" s="80"/>
+      <c r="P79" s="80"/>
+      <c r="Q79" s="81"/>
+    </row>
+    <row r="80" spans="2:17" s="36" customFormat="1" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="C79" s="73"/>
-      <c r="D79" s="73"/>
-      <c r="E79" s="73"/>
-      <c r="F79" s="73"/>
-      <c r="G79" s="73"/>
-      <c r="H79" s="73"/>
-      <c r="I79" s="73"/>
-      <c r="J79" s="73"/>
-      <c r="K79" s="73"/>
-      <c r="L79" s="73"/>
-      <c r="M79" s="73"/>
-      <c r="N79" s="73"/>
-      <c r="O79" s="73"/>
-      <c r="P79" s="73"/>
-      <c r="Q79" s="74"/>
-    </row>
-    <row r="80" spans="2:17" s="36" customFormat="1" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="76" t="s">
+      <c r="C80" s="83"/>
+      <c r="D80" s="83"/>
+      <c r="E80" s="84"/>
+      <c r="F80" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="C80" s="77"/>
-      <c r="D80" s="77"/>
-      <c r="E80" s="78"/>
-      <c r="F80" s="76" t="s">
+      <c r="G80" s="83"/>
+      <c r="H80" s="83"/>
+      <c r="I80" s="84"/>
+      <c r="J80" s="82" t="s">
         <v>22</v>
       </c>
-      <c r="G80" s="77"/>
-      <c r="H80" s="77"/>
-      <c r="I80" s="78"/>
-      <c r="J80" s="76" t="s">
+      <c r="K80" s="83"/>
+      <c r="L80" s="83"/>
+      <c r="M80" s="84"/>
+      <c r="N80" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="K80" s="77"/>
-      <c r="L80" s="77"/>
-      <c r="M80" s="78"/>
-      <c r="N80" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="O80" s="77"/>
-      <c r="P80" s="77"/>
-      <c r="Q80" s="78"/>
+      <c r="O80" s="83"/>
+      <c r="P80" s="83"/>
+      <c r="Q80" s="84"/>
     </row>
     <row r="81" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B81" s="54"/>
-      <c r="C81" s="55"/>
-      <c r="D81" s="55"/>
-      <c r="E81" s="56"/>
-      <c r="F81" s="54"/>
-      <c r="G81" s="55"/>
-      <c r="H81" s="55"/>
-      <c r="I81" s="56"/>
-      <c r="J81" s="69"/>
-      <c r="K81" s="55"/>
-      <c r="L81" s="55"/>
-      <c r="M81" s="56"/>
-      <c r="N81" s="54"/>
-      <c r="O81" s="55"/>
-      <c r="P81" s="55"/>
-      <c r="Q81" s="56"/>
+      <c r="B81" s="78"/>
+      <c r="C81" s="75"/>
+      <c r="D81" s="75"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="78"/>
+      <c r="G81" s="75"/>
+      <c r="H81" s="75"/>
+      <c r="I81" s="76"/>
+      <c r="J81" s="74"/>
+      <c r="K81" s="75"/>
+      <c r="L81" s="75"/>
+      <c r="M81" s="76"/>
+      <c r="N81" s="78"/>
+      <c r="O81" s="75"/>
+      <c r="P81" s="75"/>
+      <c r="Q81" s="76"/>
     </row>
     <row r="82" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="57"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="59"/>
-      <c r="F82" s="57"/>
-      <c r="G82" s="58"/>
-      <c r="H82" s="58"/>
-      <c r="I82" s="59"/>
-      <c r="J82" s="57"/>
-      <c r="K82" s="58"/>
-      <c r="L82" s="58"/>
-      <c r="M82" s="59"/>
-      <c r="N82" s="57"/>
-      <c r="O82" s="58"/>
-      <c r="P82" s="58"/>
-      <c r="Q82" s="59"/>
+      <c r="B82" s="77"/>
+      <c r="C82" s="65"/>
+      <c r="D82" s="65"/>
+      <c r="E82" s="66"/>
+      <c r="F82" s="77"/>
+      <c r="G82" s="65"/>
+      <c r="H82" s="65"/>
+      <c r="I82" s="66"/>
+      <c r="J82" s="77"/>
+      <c r="K82" s="65"/>
+      <c r="L82" s="65"/>
+      <c r="M82" s="66"/>
+      <c r="N82" s="77"/>
+      <c r="O82" s="65"/>
+      <c r="P82" s="65"/>
+      <c r="Q82" s="66"/>
     </row>
     <row r="83" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection password="CFAF" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="178">
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="K73:M73"/>
-    <mergeCell ref="N73:O73"/>
-    <mergeCell ref="P73:Q73"/>
-    <mergeCell ref="H69:J69"/>
-    <mergeCell ref="K69:M69"/>
-    <mergeCell ref="N69:O69"/>
-    <mergeCell ref="P69:Q69"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="J81:M82"/>
-    <mergeCell ref="N81:Q82"/>
-    <mergeCell ref="B79:Q79"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="J80:M80"/>
-    <mergeCell ref="N80:Q80"/>
-    <mergeCell ref="H74:I76"/>
-    <mergeCell ref="E74:G76"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B81:E82"/>
-    <mergeCell ref="F81:I82"/>
-    <mergeCell ref="K70:L72"/>
-    <mergeCell ref="N70:O72"/>
-    <mergeCell ref="P70:Q72"/>
-    <mergeCell ref="P74:Q76"/>
-    <mergeCell ref="N74:O76"/>
-    <mergeCell ref="K74:L76"/>
-    <mergeCell ref="H63:I65"/>
-    <mergeCell ref="E63:G65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="E70:G72"/>
-    <mergeCell ref="H70:I72"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="K59:L61"/>
-    <mergeCell ref="N59:O61"/>
-    <mergeCell ref="P59:Q61"/>
-    <mergeCell ref="P63:Q65"/>
-    <mergeCell ref="N63:O65"/>
-    <mergeCell ref="K63:L65"/>
-    <mergeCell ref="H49:I51"/>
-    <mergeCell ref="E49:G51"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E59:G61"/>
-    <mergeCell ref="H59:I61"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="K45:L47"/>
-    <mergeCell ref="N45:O47"/>
-    <mergeCell ref="P45:Q47"/>
-    <mergeCell ref="P49:Q51"/>
-    <mergeCell ref="N49:O51"/>
-    <mergeCell ref="K49:L51"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E45:G47"/>
-    <mergeCell ref="H45:I47"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="P35:Q37"/>
-    <mergeCell ref="P39:Q41"/>
-    <mergeCell ref="N39:O41"/>
-    <mergeCell ref="K39:L41"/>
-    <mergeCell ref="H39:I41"/>
-    <mergeCell ref="E39:G41"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E35:G37"/>
-    <mergeCell ref="H35:I37"/>
-    <mergeCell ref="K35:L37"/>
-    <mergeCell ref="N35:O37"/>
-    <mergeCell ref="P25:Q27"/>
-    <mergeCell ref="N25:O27"/>
-    <mergeCell ref="K25:L27"/>
-    <mergeCell ref="H25:I27"/>
-    <mergeCell ref="E25:G27"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="P14:Q16"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E21:G23"/>
-    <mergeCell ref="H21:I23"/>
-    <mergeCell ref="K21:L23"/>
-    <mergeCell ref="N21:O23"/>
-    <mergeCell ref="P21:Q23"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="K10:L12"/>
@@ -3088,7 +2917,159 @@
     <mergeCell ref="E10:G12"/>
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="P14:Q16"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E21:G23"/>
+    <mergeCell ref="H21:I23"/>
+    <mergeCell ref="K21:L23"/>
+    <mergeCell ref="N21:O23"/>
+    <mergeCell ref="P21:Q23"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E35:G37"/>
+    <mergeCell ref="H35:I37"/>
+    <mergeCell ref="K35:L37"/>
+    <mergeCell ref="N35:O37"/>
+    <mergeCell ref="P25:Q27"/>
+    <mergeCell ref="N25:O27"/>
+    <mergeCell ref="K25:L27"/>
+    <mergeCell ref="H25:I27"/>
+    <mergeCell ref="E25:G27"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="K59:L61"/>
+    <mergeCell ref="N59:O61"/>
+    <mergeCell ref="P59:Q61"/>
+    <mergeCell ref="P63:Q65"/>
+    <mergeCell ref="N63:O65"/>
+    <mergeCell ref="K63:L65"/>
+    <mergeCell ref="H49:I51"/>
+    <mergeCell ref="E49:G51"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E59:G61"/>
+    <mergeCell ref="H59:I61"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="P49:Q51"/>
+    <mergeCell ref="N49:O51"/>
+    <mergeCell ref="K49:L51"/>
+    <mergeCell ref="H63:I65"/>
+    <mergeCell ref="E63:G65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="E70:G72"/>
+    <mergeCell ref="H70:I72"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="J81:M82"/>
+    <mergeCell ref="N81:Q82"/>
+    <mergeCell ref="B79:Q79"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="J80:M80"/>
+    <mergeCell ref="N80:Q80"/>
+    <mergeCell ref="H74:I76"/>
+    <mergeCell ref="E74:G76"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B81:E82"/>
+    <mergeCell ref="F81:I82"/>
+    <mergeCell ref="P74:Q76"/>
+    <mergeCell ref="N74:O76"/>
+    <mergeCell ref="K74:L76"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="K73:M73"/>
+    <mergeCell ref="N73:O73"/>
+    <mergeCell ref="P73:Q73"/>
+    <mergeCell ref="H69:J69"/>
+    <mergeCell ref="K69:M69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="P69:Q69"/>
+    <mergeCell ref="K70:L72"/>
+    <mergeCell ref="N70:O72"/>
+    <mergeCell ref="P70:Q72"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="K45:L47"/>
+    <mergeCell ref="N45:O47"/>
+    <mergeCell ref="P45:Q47"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E45:G47"/>
+    <mergeCell ref="H45:I47"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="P35:Q37"/>
+    <mergeCell ref="P39:Q41"/>
+    <mergeCell ref="N39:O41"/>
+    <mergeCell ref="K39:L41"/>
+    <mergeCell ref="H39:I41"/>
+    <mergeCell ref="E39:G41"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:O24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -3109,7 +3090,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3124,59 +3105,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="94">
-        <f>Bracket!Q1</f>
-        <v>6</v>
-      </c>
-      <c r="C1" s="71"/>
+      <c r="B1" s="92" t="str">
+        <f>Bracket!L1 &amp; "; " &amp; Bracket!Q1</f>
+        <v xml:space="preserve">; </v>
+      </c>
+      <c r="C1" s="70"/>
       <c r="D1" s="52"/>
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
     </row>
     <row r="2" spans="1:7" ht="39" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="str">
+      <c r="A2" s="57">
         <f>Bracket!B3</f>
-        <v>Johnathan Thomas McBrides</v>
-      </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="92" t="str">
+        <v>0</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="57">
         <f>Bracket!F3</f>
-        <v>Brendan James McBride</v>
+        <v>0</v>
       </c>
       <c r="D2" s="53"/>
-      <c r="E2" s="93" t="str">
+      <c r="E2" s="58">
         <f>Bracket!J3</f>
-        <v>Some Body Else with a long</v>
+        <v>0</v>
       </c>
       <c r="F2" s="53"/>
-      <c r="G2" s="93" t="str">
+      <c r="G2" s="58">
         <f>Bracket!N3</f>
-        <v>Another long long name</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="89" t="str">
+      <c r="A3" s="54">
         <f>Bracket!B4</f>
-        <v>WR</v>
-      </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="89" t="str">
+        <v>0</v>
+      </c>
+      <c r="B3" s="55"/>
+      <c r="C3" s="54">
         <f>Bracket!F4</f>
-        <v>WR</v>
+        <v>0</v>
       </c>
       <c r="D3" s="53"/>
-      <c r="E3" s="89" t="str">
+      <c r="E3" s="54">
         <f>Bracket!J4</f>
-        <v>WR</v>
+        <v>0</v>
       </c>
       <c r="F3" s="53"/>
-      <c r="G3" s="89" t="str">
+      <c r="G3" s="54">
         <f>Bracket!N4</f>
-        <v>WR</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added a better seperation between group and mat on the second sheet
</commit_message>
<xml_diff>
--- a/Bracket.xlsx
+++ b/Bracket.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="33">
   <si>
     <t></t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>Group:</t>
-  </si>
-  <si>
-    <t>Group/Mat#</t>
   </si>
 </sst>
 </file>
@@ -510,7 +507,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -603,35 +600,67 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,46 +679,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1139,7 +1133,7 @@
   <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:Q4"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,58 +1204,58 @@
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="88"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="93"/>
-      <c r="Q3" s="94"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="62"/>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="63"/>
     </row>
     <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="97"/>
-      <c r="L4" s="97"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="95"/>
-      <c r="P4" s="95"/>
-      <c r="Q4" s="96"/>
+      <c r="B4" s="64"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="77"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="66"/>
     </row>
     <row r="5" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="84"/>
     </row>
     <row r="7" spans="1:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="60"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1281,11 +1275,11 @@
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="65"/>
-      <c r="D8" s="66"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1301,216 +1295,216 @@
       <c r="Q8" s="6"/>
     </row>
     <row r="9" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="59" t="s">
+      <c r="C9" s="72"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="59" t="s">
+      <c r="F9" s="72"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="61"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="59" t="s">
+      <c r="I9" s="72"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="61"/>
-      <c r="M9" s="60"/>
-      <c r="N9" s="59" t="s">
+      <c r="L9" s="72"/>
+      <c r="M9" s="73"/>
+      <c r="N9" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="O9" s="60"/>
-      <c r="P9" s="59" t="s">
+      <c r="O9" s="73"/>
+      <c r="P9" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q9" s="60"/>
+      <c r="Q9" s="73"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B10" s="78" t="str">
+      <c r="B10" s="58" t="str">
         <f>IF(B3="","",B3)</f>
         <v/>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="78"/>
-      <c r="I10" s="75"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="59"/>
       <c r="J10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K10" s="78"/>
-      <c r="L10" s="75"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="78"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="78"/>
-      <c r="Q10" s="76"/>
+      <c r="N10" s="58"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="58"/>
+      <c r="Q10" s="60"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B11" s="78" t="str">
+      <c r="B11" s="58" t="str">
         <f>IF(B4="","",B4)</f>
         <v/>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="78"/>
-      <c r="I11" s="75"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="58"/>
+      <c r="I11" s="59"/>
       <c r="J11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K11" s="78"/>
-      <c r="L11" s="75"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="59"/>
       <c r="M11" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N11" s="78"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="78"/>
-      <c r="Q11" s="76"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="60"/>
     </row>
     <row r="12" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="65"/>
-      <c r="G12" s="66"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="65"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="68"/>
       <c r="J12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K12" s="77"/>
-      <c r="L12" s="65"/>
+      <c r="K12" s="67"/>
+      <c r="L12" s="68"/>
       <c r="M12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N12" s="77"/>
-      <c r="O12" s="66"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="66"/>
+      <c r="N12" s="67"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="69"/>
     </row>
     <row r="13" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="59" t="s">
+      <c r="C13" s="72"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="59" t="s">
+      <c r="F13" s="72"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="61"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="59" t="s">
+      <c r="I13" s="72"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="L13" s="61"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="62" t="s">
+      <c r="L13" s="72"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="60"/>
-      <c r="P13" s="59" t="s">
+      <c r="O13" s="73"/>
+      <c r="P13" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="60"/>
+      <c r="Q13" s="73"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B14" s="78" t="str">
+      <c r="B14" s="58" t="str">
         <f>IF(F3="","",F3)</f>
         <v/>
       </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="75"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
       <c r="J14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K14" s="78"/>
-      <c r="L14" s="75"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="59"/>
       <c r="M14" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N14" s="85"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="78"/>
-      <c r="Q14" s="76"/>
+      <c r="N14" s="70"/>
+      <c r="O14" s="60"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="60"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="B15" s="78" t="str">
+      <c r="B15" s="58" t="str">
         <f>IF(F4="","",F4)</f>
         <v/>
       </c>
-      <c r="C15" s="75"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="78"/>
-      <c r="I15" s="75"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="58"/>
+      <c r="I15" s="59"/>
       <c r="J15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="78"/>
-      <c r="L15" s="75"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="59"/>
       <c r="M15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N15" s="78"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="78"/>
-      <c r="Q15" s="76"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="60"/>
     </row>
     <row r="16" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="77"/>
-      <c r="I16" s="65"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="68"/>
       <c r="J16" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K16" s="77"/>
-      <c r="L16" s="65"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="68"/>
       <c r="M16" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N16" s="77"/>
-      <c r="O16" s="66"/>
-      <c r="P16" s="77"/>
-      <c r="Q16" s="66"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="67"/>
+      <c r="Q16" s="69"/>
     </row>
     <row r="17" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="60"/>
+      <c r="C18" s="72"/>
+      <c r="D18" s="73"/>
       <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1530,11 +1524,11 @@
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="65"/>
-      <c r="D19" s="66"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="69"/>
       <c r="E19" s="4"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1550,208 +1544,208 @@
       <c r="Q19" s="6"/>
     </row>
     <row r="20" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="59" t="s">
+      <c r="B20" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="59" t="s">
+      <c r="C20" s="72"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="61"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="59" t="s">
+      <c r="F20" s="72"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="61"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="59" t="s">
+      <c r="I20" s="72"/>
+      <c r="J20" s="73"/>
+      <c r="K20" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="L20" s="61"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="59" t="s">
+      <c r="L20" s="72"/>
+      <c r="M20" s="73"/>
+      <c r="N20" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="O20" s="60"/>
-      <c r="P20" s="59" t="s">
+      <c r="O20" s="73"/>
+      <c r="P20" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q20" s="60"/>
+      <c r="Q20" s="73"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B21" s="78" t="str">
+      <c r="B21" s="58" t="str">
         <f>IF(J3="","",J3)</f>
         <v/>
       </c>
-      <c r="C21" s="75"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="78"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="76"/>
-      <c r="H21" s="78"/>
-      <c r="I21" s="75"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="59"/>
       <c r="J21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K21" s="78"/>
-      <c r="L21" s="75"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="59"/>
       <c r="M21" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N21" s="78"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="78"/>
-      <c r="Q21" s="76"/>
+      <c r="N21" s="58"/>
+      <c r="O21" s="60"/>
+      <c r="P21" s="58"/>
+      <c r="Q21" s="60"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="78" t="str">
+      <c r="B22" s="58" t="str">
         <f>IF(J4="","",J4)</f>
         <v/>
       </c>
-      <c r="C22" s="75"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="75"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="59"/>
       <c r="J22" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K22" s="78"/>
-      <c r="L22" s="75"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="59"/>
       <c r="M22" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N22" s="78"/>
-      <c r="O22" s="76"/>
-      <c r="P22" s="78"/>
-      <c r="Q22" s="76"/>
+      <c r="N22" s="58"/>
+      <c r="O22" s="60"/>
+      <c r="P22" s="58"/>
+      <c r="Q22" s="60"/>
     </row>
     <row r="23" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="65"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="68"/>
       <c r="J23" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K23" s="77"/>
-      <c r="L23" s="65"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="68"/>
       <c r="M23" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N23" s="77"/>
-      <c r="O23" s="66"/>
-      <c r="P23" s="77"/>
-      <c r="Q23" s="66"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="69"/>
+      <c r="P23" s="67"/>
+      <c r="Q23" s="69"/>
     </row>
     <row r="24" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="59" t="s">
+      <c r="C24" s="72"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="61"/>
-      <c r="G24" s="60"/>
-      <c r="H24" s="59" t="s">
+      <c r="F24" s="72"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I24" s="61"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="59" t="s">
+      <c r="I24" s="72"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="L24" s="61"/>
-      <c r="M24" s="60"/>
-      <c r="N24" s="62" t="s">
+      <c r="L24" s="72"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="O24" s="60"/>
-      <c r="P24" s="59" t="s">
+      <c r="O24" s="73"/>
+      <c r="P24" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q24" s="60"/>
+      <c r="Q24" s="73"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B25" s="78" t="str">
+      <c r="B25" s="58" t="str">
         <f>IF(N3="","",N3)</f>
         <v/>
       </c>
-      <c r="C25" s="75"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="78"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="76"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="75"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
       <c r="J25" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="78"/>
-      <c r="L25" s="75"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="59"/>
       <c r="M25" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N25" s="85"/>
-      <c r="O25" s="76"/>
-      <c r="P25" s="78"/>
-      <c r="Q25" s="76"/>
+      <c r="N25" s="70"/>
+      <c r="O25" s="60"/>
+      <c r="P25" s="58"/>
+      <c r="Q25" s="60"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B26" s="78" t="str">
+      <c r="B26" s="58" t="str">
         <f>IF(N4="","",N4)</f>
         <v/>
       </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="78"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="78"/>
-      <c r="I26" s="75"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
       <c r="J26" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="78"/>
-      <c r="L26" s="75"/>
+      <c r="K26" s="58"/>
+      <c r="L26" s="59"/>
       <c r="M26" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="78"/>
-      <c r="O26" s="76"/>
-      <c r="P26" s="78"/>
-      <c r="Q26" s="76"/>
+      <c r="N26" s="58"/>
+      <c r="O26" s="60"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="60"/>
     </row>
     <row r="27" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="77"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="65"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="68"/>
       <c r="J27" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K27" s="77"/>
-      <c r="L27" s="65"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="68"/>
       <c r="M27" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="77"/>
-      <c r="O27" s="66"/>
-      <c r="P27" s="77"/>
-      <c r="Q27" s="66"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="67"/>
+      <c r="Q27" s="69"/>
     </row>
     <row r="28" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
@@ -1789,18 +1783,18 @@
     </row>
     <row r="30" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="68" t="s">
+      <c r="B31" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="69"/>
-      <c r="D31" s="70"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="84"/>
     </row>
     <row r="32" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="61"/>
-      <c r="D32" s="60"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="18" t="s">
         <v>8</v>
       </c>
@@ -1820,11 +1814,11 @@
       <c r="Q32" s="17"/>
     </row>
     <row r="33" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="64" t="s">
+      <c r="B33" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="65"/>
-      <c r="D33" s="66"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="69"/>
       <c r="E33" s="20"/>
       <c r="F33" s="21"/>
       <c r="G33" s="21"/>
@@ -1840,215 +1834,215 @@
       <c r="Q33" s="22"/>
     </row>
     <row r="34" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="63" t="s">
+      <c r="B34" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="C34" s="61"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="63" t="s">
+      <c r="C34" s="72"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="61"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="63" t="s">
+      <c r="F34" s="72"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="I34" s="61"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="63" t="s">
+      <c r="I34" s="72"/>
+      <c r="J34" s="73"/>
+      <c r="K34" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="L34" s="61"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="63" t="s">
+      <c r="L34" s="72"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="O34" s="60"/>
-      <c r="P34" s="63" t="s">
+      <c r="O34" s="73"/>
+      <c r="P34" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q34" s="60"/>
+      <c r="Q34" s="73"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B35" s="86" t="str">
+      <c r="B35" s="81" t="str">
         <f>IF(B3="","",B3)</f>
         <v/>
       </c>
-      <c r="C35" s="75"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="75"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="81"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="81"/>
+      <c r="I35" s="59"/>
       <c r="J35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="86"/>
-      <c r="L35" s="75"/>
+      <c r="K35" s="81"/>
+      <c r="L35" s="59"/>
       <c r="M35" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N35" s="86"/>
-      <c r="O35" s="76"/>
-      <c r="P35" s="86"/>
-      <c r="Q35" s="76"/>
+      <c r="N35" s="81"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="60"/>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B36" s="86" t="str">
+      <c r="B36" s="81" t="str">
         <f>IF(B4="","",B4)</f>
         <v/>
       </c>
-      <c r="C36" s="75"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="78"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="78"/>
-      <c r="I36" s="75"/>
+      <c r="C36" s="59"/>
+      <c r="D36" s="60"/>
+      <c r="E36" s="58"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="60"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="59"/>
       <c r="J36" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K36" s="78"/>
-      <c r="L36" s="75"/>
+      <c r="K36" s="58"/>
+      <c r="L36" s="59"/>
       <c r="M36" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N36" s="78"/>
-      <c r="O36" s="76"/>
-      <c r="P36" s="78"/>
-      <c r="Q36" s="76"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="58"/>
+      <c r="Q36" s="60"/>
     </row>
     <row r="37" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="20"/>
       <c r="C37" s="21"/>
       <c r="D37" s="22"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="65"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="68"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="68"/>
       <c r="J37" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="K37" s="77"/>
-      <c r="L37" s="65"/>
+      <c r="K37" s="67"/>
+      <c r="L37" s="68"/>
       <c r="M37" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="N37" s="77"/>
-      <c r="O37" s="66"/>
-      <c r="P37" s="77"/>
-      <c r="Q37" s="66"/>
+      <c r="N37" s="67"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="67"/>
+      <c r="Q37" s="69"/>
     </row>
     <row r="38" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="63" t="s">
+      <c r="B38" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="61"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="63" t="s">
+      <c r="C38" s="72"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="61"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="63" t="s">
+      <c r="F38" s="72"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="I38" s="61"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="63" t="s">
+      <c r="I38" s="72"/>
+      <c r="J38" s="73"/>
+      <c r="K38" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="L38" s="61"/>
-      <c r="M38" s="60"/>
-      <c r="N38" s="73" t="s">
+      <c r="L38" s="72"/>
+      <c r="M38" s="73"/>
+      <c r="N38" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="O38" s="60"/>
-      <c r="P38" s="63" t="s">
+      <c r="O38" s="73"/>
+      <c r="P38" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q38" s="60"/>
+      <c r="Q38" s="73"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B39" s="86" t="str">
+      <c r="B39" s="81" t="str">
         <f>IF(J3="","",J3)</f>
         <v/>
       </c>
-      <c r="C39" s="75"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="86"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="86"/>
-      <c r="I39" s="75"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="60"/>
+      <c r="E39" s="81"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="81"/>
+      <c r="I39" s="59"/>
       <c r="J39" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K39" s="86"/>
-      <c r="L39" s="75"/>
+      <c r="K39" s="81"/>
+      <c r="L39" s="59"/>
       <c r="M39" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N39" s="87"/>
-      <c r="O39" s="76"/>
-      <c r="P39" s="86"/>
-      <c r="Q39" s="76"/>
+      <c r="N39" s="85"/>
+      <c r="O39" s="60"/>
+      <c r="P39" s="81"/>
+      <c r="Q39" s="60"/>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B40" s="86" t="str">
+      <c r="B40" s="81" t="str">
         <f>IF(J4="","",J4)</f>
         <v/>
       </c>
-      <c r="C40" s="75"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="78"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="78"/>
-      <c r="I40" s="75"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="59"/>
+      <c r="G40" s="60"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="59"/>
       <c r="J40" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K40" s="78"/>
-      <c r="L40" s="75"/>
+      <c r="K40" s="58"/>
+      <c r="L40" s="59"/>
       <c r="M40" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N40" s="78"/>
-      <c r="O40" s="76"/>
-      <c r="P40" s="78"/>
-      <c r="Q40" s="76"/>
+      <c r="N40" s="58"/>
+      <c r="O40" s="60"/>
+      <c r="P40" s="58"/>
+      <c r="Q40" s="60"/>
     </row>
     <row r="41" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B41" s="20"/>
       <c r="C41" s="21"/>
       <c r="D41" s="22"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="65"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="69"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="68"/>
       <c r="J41" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="K41" s="77"/>
-      <c r="L41" s="65"/>
+      <c r="K41" s="67"/>
+      <c r="L41" s="68"/>
       <c r="M41" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="N41" s="77"/>
-      <c r="O41" s="66"/>
-      <c r="P41" s="77"/>
-      <c r="Q41" s="66"/>
+      <c r="N41" s="67"/>
+      <c r="O41" s="69"/>
+      <c r="P41" s="67"/>
+      <c r="Q41" s="69"/>
     </row>
     <row r="42" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="61"/>
-      <c r="D42" s="60"/>
+      <c r="C42" s="72"/>
+      <c r="D42" s="73"/>
       <c r="E42" s="25" t="s">
         <v>8</v>
       </c>
@@ -2068,11 +2062,11 @@
       <c r="Q42" s="26"/>
     </row>
     <row r="43" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C43" s="65"/>
-      <c r="D43" s="66"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="69"/>
       <c r="E43" s="20"/>
       <c r="F43" s="21"/>
       <c r="G43" s="21"/>
@@ -2088,208 +2082,208 @@
       <c r="Q43" s="22"/>
     </row>
     <row r="44" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="63" t="s">
+      <c r="B44" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="61"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="63" t="s">
+      <c r="C44" s="72"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="F44" s="61"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="63" t="s">
+      <c r="F44" s="72"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="I44" s="61"/>
-      <c r="J44" s="60"/>
-      <c r="K44" s="63" t="s">
+      <c r="I44" s="72"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="L44" s="61"/>
-      <c r="M44" s="60"/>
-      <c r="N44" s="63" t="s">
+      <c r="L44" s="72"/>
+      <c r="M44" s="73"/>
+      <c r="N44" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="O44" s="60"/>
-      <c r="P44" s="63" t="s">
+      <c r="O44" s="73"/>
+      <c r="P44" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q44" s="60"/>
+      <c r="Q44" s="73"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B45" s="86" t="str">
+      <c r="B45" s="81" t="str">
         <f>IF(F3="","",F3)</f>
         <v/>
       </c>
-      <c r="C45" s="75"/>
-      <c r="D45" s="76"/>
-      <c r="E45" s="86"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="76"/>
-      <c r="H45" s="86"/>
-      <c r="I45" s="75"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="60"/>
+      <c r="H45" s="81"/>
+      <c r="I45" s="59"/>
       <c r="J45" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K45" s="86"/>
-      <c r="L45" s="75"/>
+      <c r="K45" s="81"/>
+      <c r="L45" s="59"/>
       <c r="M45" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N45" s="86"/>
-      <c r="O45" s="76"/>
-      <c r="P45" s="86"/>
-      <c r="Q45" s="76"/>
+      <c r="N45" s="81"/>
+      <c r="O45" s="60"/>
+      <c r="P45" s="81"/>
+      <c r="Q45" s="60"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B46" s="86" t="str">
+      <c r="B46" s="81" t="str">
         <f>IF(F4="","",F4)</f>
         <v/>
       </c>
-      <c r="C46" s="75"/>
-      <c r="D46" s="76"/>
-      <c r="E46" s="78"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="78"/>
-      <c r="I46" s="75"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="59"/>
       <c r="J46" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K46" s="78"/>
-      <c r="L46" s="75"/>
+      <c r="K46" s="58"/>
+      <c r="L46" s="59"/>
       <c r="M46" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N46" s="78"/>
-      <c r="O46" s="76"/>
-      <c r="P46" s="78"/>
-      <c r="Q46" s="76"/>
+      <c r="N46" s="58"/>
+      <c r="O46" s="60"/>
+      <c r="P46" s="58"/>
+      <c r="Q46" s="60"/>
     </row>
     <row r="47" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B47" s="20"/>
       <c r="C47" s="21"/>
       <c r="D47" s="22"/>
-      <c r="E47" s="77"/>
-      <c r="F47" s="65"/>
-      <c r="G47" s="66"/>
-      <c r="H47" s="77"/>
-      <c r="I47" s="65"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="68"/>
       <c r="J47" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="K47" s="77"/>
-      <c r="L47" s="65"/>
+      <c r="K47" s="67"/>
+      <c r="L47" s="68"/>
       <c r="M47" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="N47" s="77"/>
-      <c r="O47" s="66"/>
-      <c r="P47" s="77"/>
-      <c r="Q47" s="66"/>
+      <c r="N47" s="67"/>
+      <c r="O47" s="69"/>
+      <c r="P47" s="67"/>
+      <c r="Q47" s="69"/>
     </row>
     <row r="48" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="63" t="s">
+      <c r="B48" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="63" t="s">
+      <c r="C48" s="72"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="61"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="63" t="s">
+      <c r="F48" s="72"/>
+      <c r="G48" s="73"/>
+      <c r="H48" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="I48" s="61"/>
-      <c r="J48" s="60"/>
-      <c r="K48" s="63" t="s">
+      <c r="I48" s="72"/>
+      <c r="J48" s="73"/>
+      <c r="K48" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="L48" s="61"/>
-      <c r="M48" s="60"/>
-      <c r="N48" s="73" t="s">
+      <c r="L48" s="72"/>
+      <c r="M48" s="73"/>
+      <c r="N48" s="96" t="s">
         <v>13</v>
       </c>
-      <c r="O48" s="60"/>
-      <c r="P48" s="63" t="s">
+      <c r="O48" s="73"/>
+      <c r="P48" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="Q48" s="60"/>
+      <c r="Q48" s="73"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B49" s="86" t="str">
+      <c r="B49" s="81" t="str">
         <f>IF(N3="","",N3)</f>
         <v/>
       </c>
-      <c r="C49" s="75"/>
-      <c r="D49" s="76"/>
-      <c r="E49" s="86"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="76"/>
-      <c r="H49" s="86"/>
-      <c r="I49" s="75"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="60"/>
+      <c r="E49" s="81"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="60"/>
+      <c r="H49" s="81"/>
+      <c r="I49" s="59"/>
       <c r="J49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="K49" s="86"/>
-      <c r="L49" s="75"/>
+      <c r="K49" s="81"/>
+      <c r="L49" s="59"/>
       <c r="M49" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N49" s="87"/>
-      <c r="O49" s="76"/>
-      <c r="P49" s="86"/>
-      <c r="Q49" s="76"/>
+      <c r="N49" s="85"/>
+      <c r="O49" s="60"/>
+      <c r="P49" s="81"/>
+      <c r="Q49" s="60"/>
     </row>
     <row r="50" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B50" s="86" t="str">
+      <c r="B50" s="81" t="str">
         <f>IF(N4="","",N4)</f>
         <v/>
       </c>
-      <c r="C50" s="75"/>
-      <c r="D50" s="76"/>
-      <c r="E50" s="78"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="78"/>
-      <c r="I50" s="75"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="60"/>
+      <c r="E50" s="58"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="60"/>
+      <c r="H50" s="58"/>
+      <c r="I50" s="59"/>
       <c r="J50" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="K50" s="78"/>
-      <c r="L50" s="75"/>
+      <c r="K50" s="58"/>
+      <c r="L50" s="59"/>
       <c r="M50" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="N50" s="78"/>
-      <c r="O50" s="76"/>
-      <c r="P50" s="78"/>
-      <c r="Q50" s="76"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="60"/>
     </row>
     <row r="51" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B51" s="20"/>
       <c r="C51" s="21"/>
       <c r="D51" s="22"/>
-      <c r="E51" s="77"/>
-      <c r="F51" s="65"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="77"/>
-      <c r="I51" s="65"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="68"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="67"/>
+      <c r="I51" s="68"/>
       <c r="J51" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="K51" s="77"/>
-      <c r="L51" s="65"/>
+      <c r="K51" s="67"/>
+      <c r="L51" s="68"/>
       <c r="M51" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="N51" s="77"/>
-      <c r="O51" s="66"/>
-      <c r="P51" s="77"/>
-      <c r="Q51" s="66"/>
+      <c r="N51" s="67"/>
+      <c r="O51" s="69"/>
+      <c r="P51" s="67"/>
+      <c r="Q51" s="69"/>
     </row>
     <row r="52" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C52"/>
@@ -2301,18 +2295,18 @@
     </row>
     <row r="54" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="68" t="s">
+      <c r="B55" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="C55" s="69"/>
-      <c r="D55" s="70"/>
+      <c r="C55" s="83"/>
+      <c r="D55" s="84"/>
     </row>
     <row r="56" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="71" t="s">
+      <c r="B56" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C56" s="61"/>
-      <c r="D56" s="60"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="73"/>
       <c r="E56" s="1" t="s">
         <v>8</v>
       </c>
@@ -2332,11 +2326,11 @@
       <c r="Q56" s="3"/>
     </row>
     <row r="57" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="72" t="s">
+      <c r="B57" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="65"/>
-      <c r="D57" s="66"/>
+      <c r="C57" s="68"/>
+      <c r="D57" s="69"/>
       <c r="E57" s="4"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
@@ -2352,11 +2346,11 @@
       <c r="Q57" s="6"/>
     </row>
     <row r="58" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="59" t="s">
+      <c r="B58" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="61"/>
-      <c r="D58" s="60"/>
+      <c r="C58" s="72"/>
+      <c r="D58" s="73"/>
       <c r="E58" s="2" t="s">
         <v>10</v>
       </c>
@@ -2382,83 +2376,83 @@
       <c r="Q58" s="3"/>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B59" s="78" t="str">
+      <c r="B59" s="58" t="str">
         <f>IF(B3="","",B3)</f>
         <v/>
       </c>
-      <c r="C59" s="75"/>
-      <c r="D59" s="76"/>
-      <c r="E59" s="78"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="76"/>
-      <c r="H59" s="78"/>
-      <c r="I59" s="75"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="60"/>
+      <c r="E59" s="58"/>
+      <c r="F59" s="59"/>
+      <c r="G59" s="60"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="59"/>
       <c r="J59" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K59" s="78"/>
-      <c r="L59" s="75"/>
+      <c r="K59" s="58"/>
+      <c r="L59" s="59"/>
       <c r="M59" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N59" s="78"/>
-      <c r="O59" s="76"/>
-      <c r="P59" s="78"/>
-      <c r="Q59" s="76"/>
+      <c r="N59" s="58"/>
+      <c r="O59" s="60"/>
+      <c r="P59" s="58"/>
+      <c r="Q59" s="60"/>
     </row>
     <row r="60" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B60" s="78" t="str">
+      <c r="B60" s="58" t="str">
         <f>IF(B4="","",B4)</f>
         <v/>
       </c>
-      <c r="C60" s="75"/>
-      <c r="D60" s="76"/>
-      <c r="E60" s="78"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="76"/>
-      <c r="H60" s="78"/>
-      <c r="I60" s="75"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="60"/>
+      <c r="E60" s="58"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="60"/>
+      <c r="H60" s="58"/>
+      <c r="I60" s="59"/>
       <c r="J60" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K60" s="78"/>
-      <c r="L60" s="75"/>
+      <c r="K60" s="58"/>
+      <c r="L60" s="59"/>
       <c r="M60" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N60" s="78"/>
-      <c r="O60" s="76"/>
-      <c r="P60" s="78"/>
-      <c r="Q60" s="76"/>
+      <c r="N60" s="58"/>
+      <c r="O60" s="60"/>
+      <c r="P60" s="58"/>
+      <c r="Q60" s="60"/>
     </row>
     <row r="61" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4"/>
       <c r="C61" s="5"/>
       <c r="D61" s="6"/>
-      <c r="E61" s="77"/>
-      <c r="F61" s="65"/>
-      <c r="G61" s="66"/>
-      <c r="H61" s="77"/>
-      <c r="I61" s="65"/>
+      <c r="E61" s="67"/>
+      <c r="F61" s="68"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="67"/>
+      <c r="I61" s="68"/>
       <c r="J61" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K61" s="77"/>
-      <c r="L61" s="65"/>
+      <c r="K61" s="67"/>
+      <c r="L61" s="68"/>
       <c r="M61" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N61" s="77"/>
-      <c r="O61" s="66"/>
-      <c r="P61" s="77"/>
-      <c r="Q61" s="66"/>
+      <c r="N61" s="67"/>
+      <c r="O61" s="69"/>
+      <c r="P61" s="67"/>
+      <c r="Q61" s="69"/>
     </row>
     <row r="62" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="59" t="s">
+      <c r="B62" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="60"/>
+      <c r="C62" s="72"/>
+      <c r="D62" s="73"/>
       <c r="E62" s="2" t="s">
         <v>10</v>
       </c>
@@ -2484,84 +2478,84 @@
       <c r="Q62" s="3"/>
     </row>
     <row r="63" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B63" s="78" t="str">
+      <c r="B63" s="58" t="str">
         <f>IF(N3="","",N3)</f>
         <v/>
       </c>
-      <c r="C63" s="75"/>
-      <c r="D63" s="76"/>
-      <c r="E63" s="78"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="76"/>
-      <c r="H63" s="78"/>
-      <c r="I63" s="75"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="60"/>
+      <c r="E63" s="58"/>
+      <c r="F63" s="59"/>
+      <c r="G63" s="60"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="59"/>
       <c r="J63" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K63" s="78"/>
-      <c r="L63" s="75"/>
+      <c r="K63" s="58"/>
+      <c r="L63" s="59"/>
       <c r="M63" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N63" s="85"/>
-      <c r="O63" s="76"/>
-      <c r="P63" s="78"/>
-      <c r="Q63" s="76"/>
+      <c r="N63" s="70"/>
+      <c r="O63" s="60"/>
+      <c r="P63" s="58"/>
+      <c r="Q63" s="60"/>
     </row>
     <row r="64" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B64" s="78" t="str">
+      <c r="B64" s="58" t="str">
         <f>IF(N4="","",N4)</f>
         <v/>
       </c>
-      <c r="C64" s="75"/>
-      <c r="D64" s="76"/>
-      <c r="E64" s="78"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="76"/>
-      <c r="H64" s="78"/>
-      <c r="I64" s="75"/>
+      <c r="C64" s="59"/>
+      <c r="D64" s="60"/>
+      <c r="E64" s="58"/>
+      <c r="F64" s="59"/>
+      <c r="G64" s="60"/>
+      <c r="H64" s="58"/>
+      <c r="I64" s="59"/>
       <c r="J64" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K64" s="78"/>
-      <c r="L64" s="75"/>
+      <c r="K64" s="58"/>
+      <c r="L64" s="59"/>
       <c r="M64" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N64" s="78"/>
-      <c r="O64" s="76"/>
-      <c r="P64" s="78"/>
-      <c r="Q64" s="76"/>
+      <c r="N64" s="58"/>
+      <c r="O64" s="60"/>
+      <c r="P64" s="58"/>
+      <c r="Q64" s="60"/>
     </row>
     <row r="65" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4"/>
       <c r="C65" s="5"/>
       <c r="D65" s="6"/>
-      <c r="E65" s="77"/>
-      <c r="F65" s="65"/>
-      <c r="G65" s="66"/>
-      <c r="H65" s="77"/>
-      <c r="I65" s="65"/>
+      <c r="E65" s="67"/>
+      <c r="F65" s="68"/>
+      <c r="G65" s="69"/>
+      <c r="H65" s="67"/>
+      <c r="I65" s="68"/>
       <c r="J65" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K65" s="77"/>
-      <c r="L65" s="65"/>
+      <c r="K65" s="67"/>
+      <c r="L65" s="68"/>
       <c r="M65" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N65" s="77"/>
-      <c r="O65" s="66"/>
-      <c r="P65" s="77"/>
-      <c r="Q65" s="66"/>
+      <c r="N65" s="67"/>
+      <c r="O65" s="69"/>
+      <c r="P65" s="67"/>
+      <c r="Q65" s="69"/>
     </row>
     <row r="66" spans="2:17" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="67" spans="2:17" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="71" t="s">
+      <c r="B67" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C67" s="61"/>
-      <c r="D67" s="60"/>
+      <c r="C67" s="72"/>
+      <c r="D67" s="73"/>
       <c r="E67" s="1" t="s">
         <v>8</v>
       </c>
@@ -2581,11 +2575,11 @@
       <c r="Q67" s="3"/>
     </row>
     <row r="68" spans="2:17" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="72" t="s">
+      <c r="B68" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="C68" s="65"/>
-      <c r="D68" s="66"/>
+      <c r="C68" s="68"/>
+      <c r="D68" s="69"/>
       <c r="E68" s="4"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
@@ -2601,297 +2595,451 @@
       <c r="Q68" s="6"/>
     </row>
     <row r="69" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="59" t="s">
+      <c r="B69" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="C69" s="61"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="59" t="s">
+      <c r="C69" s="72"/>
+      <c r="D69" s="73"/>
+      <c r="E69" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F69" s="61"/>
-      <c r="G69" s="60"/>
-      <c r="H69" s="59" t="s">
+      <c r="F69" s="72"/>
+      <c r="G69" s="73"/>
+      <c r="H69" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I69" s="61"/>
-      <c r="J69" s="60"/>
-      <c r="K69" s="59" t="s">
+      <c r="I69" s="72"/>
+      <c r="J69" s="73"/>
+      <c r="K69" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="L69" s="61"/>
-      <c r="M69" s="60"/>
-      <c r="N69" s="59" t="s">
+      <c r="L69" s="72"/>
+      <c r="M69" s="73"/>
+      <c r="N69" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="O69" s="60"/>
-      <c r="P69" s="59" t="s">
+      <c r="O69" s="73"/>
+      <c r="P69" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q69" s="60"/>
+      <c r="Q69" s="73"/>
     </row>
     <row r="70" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B70" s="78" t="str">
+      <c r="B70" s="58" t="str">
         <f>IF(F3="","",F3)</f>
         <v/>
       </c>
-      <c r="C70" s="75"/>
-      <c r="D70" s="76"/>
-      <c r="E70" s="78"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="76"/>
-      <c r="H70" s="78"/>
-      <c r="I70" s="75"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="60"/>
+      <c r="E70" s="58"/>
+      <c r="F70" s="59"/>
+      <c r="G70" s="60"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="59"/>
       <c r="J70" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K70" s="78"/>
-      <c r="L70" s="75"/>
+      <c r="K70" s="58"/>
+      <c r="L70" s="59"/>
       <c r="M70" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N70" s="78"/>
-      <c r="O70" s="76"/>
-      <c r="P70" s="78"/>
-      <c r="Q70" s="76"/>
+      <c r="N70" s="58"/>
+      <c r="O70" s="60"/>
+      <c r="P70" s="58"/>
+      <c r="Q70" s="60"/>
     </row>
     <row r="71" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B71" s="78" t="str">
+      <c r="B71" s="58" t="str">
         <f>IF(F4="","",F4)</f>
         <v/>
       </c>
-      <c r="C71" s="75"/>
-      <c r="D71" s="76"/>
-      <c r="E71" s="78"/>
-      <c r="F71" s="75"/>
-      <c r="G71" s="76"/>
-      <c r="H71" s="78"/>
-      <c r="I71" s="75"/>
+      <c r="C71" s="59"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="59"/>
       <c r="J71" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K71" s="78"/>
-      <c r="L71" s="75"/>
+      <c r="K71" s="58"/>
+      <c r="L71" s="59"/>
       <c r="M71" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N71" s="78"/>
-      <c r="O71" s="76"/>
-      <c r="P71" s="78"/>
-      <c r="Q71" s="76"/>
+      <c r="N71" s="58"/>
+      <c r="O71" s="60"/>
+      <c r="P71" s="58"/>
+      <c r="Q71" s="60"/>
     </row>
     <row r="72" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B72" s="4"/>
       <c r="C72" s="5"/>
       <c r="D72" s="6"/>
-      <c r="E72" s="77"/>
-      <c r="F72" s="65"/>
-      <c r="G72" s="66"/>
-      <c r="H72" s="77"/>
-      <c r="I72" s="65"/>
+      <c r="E72" s="67"/>
+      <c r="F72" s="68"/>
+      <c r="G72" s="69"/>
+      <c r="H72" s="67"/>
+      <c r="I72" s="68"/>
       <c r="J72" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K72" s="77"/>
-      <c r="L72" s="65"/>
+      <c r="K72" s="67"/>
+      <c r="L72" s="68"/>
       <c r="M72" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="N72" s="77"/>
-      <c r="O72" s="66"/>
-      <c r="P72" s="77"/>
-      <c r="Q72" s="66"/>
+      <c r="N72" s="67"/>
+      <c r="O72" s="69"/>
+      <c r="P72" s="67"/>
+      <c r="Q72" s="69"/>
     </row>
     <row r="73" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="59" t="s">
+      <c r="B73" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C73" s="61"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="59" t="s">
+      <c r="C73" s="72"/>
+      <c r="D73" s="73"/>
+      <c r="E73" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="F73" s="61"/>
-      <c r="G73" s="60"/>
-      <c r="H73" s="59" t="s">
+      <c r="F73" s="72"/>
+      <c r="G73" s="73"/>
+      <c r="H73" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="I73" s="61"/>
-      <c r="J73" s="60"/>
-      <c r="K73" s="59" t="s">
+      <c r="I73" s="72"/>
+      <c r="J73" s="73"/>
+      <c r="K73" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="L73" s="61"/>
-      <c r="M73" s="60"/>
-      <c r="N73" s="62" t="s">
+      <c r="L73" s="72"/>
+      <c r="M73" s="73"/>
+      <c r="N73" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="O73" s="60"/>
-      <c r="P73" s="59" t="s">
+      <c r="O73" s="73"/>
+      <c r="P73" s="71" t="s">
         <v>14</v>
       </c>
-      <c r="Q73" s="60"/>
+      <c r="Q73" s="73"/>
     </row>
     <row r="74" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B74" s="78" t="str">
+      <c r="B74" s="58" t="str">
         <f>IF(J3="","",J3)</f>
         <v/>
       </c>
-      <c r="C74" s="75"/>
-      <c r="D74" s="76"/>
-      <c r="E74" s="78"/>
-      <c r="F74" s="75"/>
-      <c r="G74" s="76"/>
-      <c r="H74" s="78"/>
-      <c r="I74" s="75"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="60"/>
+      <c r="E74" s="58"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="60"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="59"/>
       <c r="J74" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K74" s="78"/>
-      <c r="L74" s="75"/>
+      <c r="K74" s="58"/>
+      <c r="L74" s="59"/>
       <c r="M74" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="N74" s="85"/>
-      <c r="O74" s="76"/>
-      <c r="P74" s="78"/>
-      <c r="Q74" s="76"/>
+      <c r="N74" s="70"/>
+      <c r="O74" s="60"/>
+      <c r="P74" s="58"/>
+      <c r="Q74" s="60"/>
     </row>
     <row r="75" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B75" s="78" t="str">
+      <c r="B75" s="58" t="str">
         <f>IF(J4="","",J4)</f>
         <v/>
       </c>
-      <c r="C75" s="75"/>
-      <c r="D75" s="76"/>
-      <c r="E75" s="78"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="76"/>
-      <c r="H75" s="78"/>
-      <c r="I75" s="75"/>
+      <c r="C75" s="59"/>
+      <c r="D75" s="60"/>
+      <c r="E75" s="58"/>
+      <c r="F75" s="59"/>
+      <c r="G75" s="60"/>
+      <c r="H75" s="58"/>
+      <c r="I75" s="59"/>
       <c r="J75" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K75" s="78"/>
-      <c r="L75" s="75"/>
+      <c r="K75" s="58"/>
+      <c r="L75" s="59"/>
       <c r="M75" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="N75" s="78"/>
-      <c r="O75" s="76"/>
-      <c r="P75" s="78"/>
-      <c r="Q75" s="76"/>
+      <c r="N75" s="58"/>
+      <c r="O75" s="60"/>
+      <c r="P75" s="58"/>
+      <c r="Q75" s="60"/>
     </row>
     <row r="76" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4"/>
       <c r="C76" s="5"/>
       <c r="D76" s="6"/>
-      <c r="E76" s="77"/>
-      <c r="F76" s="65"/>
-      <c r="G76" s="66"/>
-      <c r="H76" s="77"/>
-      <c r="I76" s="65"/>
+      <c r="E76" s="67"/>
+      <c r="F76" s="68"/>
+      <c r="G76" s="69"/>
+      <c r="H76" s="67"/>
+      <c r="I76" s="68"/>
       <c r="J76" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="K76" s="77"/>
-      <c r="L76" s="65"/>
+      <c r="K76" s="67"/>
+      <c r="L76" s="68"/>
       <c r="M76" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="N76" s="77"/>
-      <c r="O76" s="66"/>
-      <c r="P76" s="77"/>
-      <c r="Q76" s="66"/>
+      <c r="N76" s="67"/>
+      <c r="O76" s="69"/>
+      <c r="P76" s="67"/>
+      <c r="Q76" s="69"/>
     </row>
     <row r="77" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="78" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="2:17" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="79" t="s">
+      <c r="B79" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C79" s="80"/>
-      <c r="D79" s="80"/>
-      <c r="E79" s="80"/>
-      <c r="F79" s="80"/>
-      <c r="G79" s="80"/>
-      <c r="H79" s="80"/>
-      <c r="I79" s="80"/>
-      <c r="J79" s="80"/>
-      <c r="K79" s="80"/>
-      <c r="L79" s="80"/>
-      <c r="M79" s="80"/>
-      <c r="N79" s="80"/>
-      <c r="O79" s="80"/>
-      <c r="P79" s="80"/>
-      <c r="Q79" s="81"/>
+      <c r="C79" s="88"/>
+      <c r="D79" s="88"/>
+      <c r="E79" s="88"/>
+      <c r="F79" s="88"/>
+      <c r="G79" s="88"/>
+      <c r="H79" s="88"/>
+      <c r="I79" s="88"/>
+      <c r="J79" s="88"/>
+      <c r="K79" s="88"/>
+      <c r="L79" s="88"/>
+      <c r="M79" s="88"/>
+      <c r="N79" s="88"/>
+      <c r="O79" s="88"/>
+      <c r="P79" s="88"/>
+      <c r="Q79" s="89"/>
     </row>
     <row r="80" spans="2:17" s="36" customFormat="1" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="82" t="s">
+      <c r="B80" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C80" s="83"/>
-      <c r="D80" s="83"/>
-      <c r="E80" s="84"/>
-      <c r="F80" s="82" t="s">
+      <c r="C80" s="91"/>
+      <c r="D80" s="91"/>
+      <c r="E80" s="92"/>
+      <c r="F80" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="G80" s="83"/>
-      <c r="H80" s="83"/>
-      <c r="I80" s="84"/>
-      <c r="J80" s="82" t="s">
+      <c r="G80" s="91"/>
+      <c r="H80" s="91"/>
+      <c r="I80" s="92"/>
+      <c r="J80" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="K80" s="83"/>
-      <c r="L80" s="83"/>
-      <c r="M80" s="84"/>
-      <c r="N80" s="82" t="s">
+      <c r="K80" s="91"/>
+      <c r="L80" s="91"/>
+      <c r="M80" s="92"/>
+      <c r="N80" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="O80" s="83"/>
-      <c r="P80" s="83"/>
-      <c r="Q80" s="84"/>
+      <c r="O80" s="91"/>
+      <c r="P80" s="91"/>
+      <c r="Q80" s="92"/>
     </row>
     <row r="81" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B81" s="78"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="76"/>
-      <c r="F81" s="78"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="I81" s="76"/>
-      <c r="J81" s="74"/>
-      <c r="K81" s="75"/>
-      <c r="L81" s="75"/>
-      <c r="M81" s="76"/>
-      <c r="N81" s="78"/>
-      <c r="O81" s="75"/>
-      <c r="P81" s="75"/>
-      <c r="Q81" s="76"/>
+      <c r="B81" s="58"/>
+      <c r="C81" s="59"/>
+      <c r="D81" s="59"/>
+      <c r="E81" s="60"/>
+      <c r="F81" s="58"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="59"/>
+      <c r="I81" s="60"/>
+      <c r="J81" s="86"/>
+      <c r="K81" s="59"/>
+      <c r="L81" s="59"/>
+      <c r="M81" s="60"/>
+      <c r="N81" s="58"/>
+      <c r="O81" s="59"/>
+      <c r="P81" s="59"/>
+      <c r="Q81" s="60"/>
     </row>
     <row r="82" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="77"/>
-      <c r="C82" s="65"/>
-      <c r="D82" s="65"/>
-      <c r="E82" s="66"/>
-      <c r="F82" s="77"/>
-      <c r="G82" s="65"/>
-      <c r="H82" s="65"/>
-      <c r="I82" s="66"/>
-      <c r="J82" s="77"/>
-      <c r="K82" s="65"/>
-      <c r="L82" s="65"/>
-      <c r="M82" s="66"/>
-      <c r="N82" s="77"/>
-      <c r="O82" s="65"/>
-      <c r="P82" s="65"/>
-      <c r="Q82" s="66"/>
+      <c r="B82" s="67"/>
+      <c r="C82" s="68"/>
+      <c r="D82" s="68"/>
+      <c r="E82" s="69"/>
+      <c r="F82" s="67"/>
+      <c r="G82" s="68"/>
+      <c r="H82" s="68"/>
+      <c r="I82" s="69"/>
+      <c r="J82" s="67"/>
+      <c r="K82" s="68"/>
+      <c r="L82" s="68"/>
+      <c r="M82" s="69"/>
+      <c r="N82" s="67"/>
+      <c r="O82" s="68"/>
+      <c r="P82" s="68"/>
+      <c r="Q82" s="69"/>
     </row>
     <row r="83" spans="2:17" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection password="CFAF" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="178">
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="P39:Q41"/>
+    <mergeCell ref="N39:O41"/>
+    <mergeCell ref="K39:L41"/>
+    <mergeCell ref="H39:I41"/>
+    <mergeCell ref="E39:G41"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="K38:M38"/>
+    <mergeCell ref="P24:Q24"/>
+    <mergeCell ref="P20:Q20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="E48:G48"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E45:G47"/>
+    <mergeCell ref="H45:I47"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:J44"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E13:G13"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="K44:M44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="P44:Q44"/>
+    <mergeCell ref="P48:Q48"/>
+    <mergeCell ref="N48:O48"/>
+    <mergeCell ref="K48:M48"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="K34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="K45:L47"/>
+    <mergeCell ref="N45:O47"/>
+    <mergeCell ref="P45:Q47"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="N73:O73"/>
+    <mergeCell ref="P73:Q73"/>
+    <mergeCell ref="H69:J69"/>
+    <mergeCell ref="K69:M69"/>
+    <mergeCell ref="N69:O69"/>
+    <mergeCell ref="P69:Q69"/>
+    <mergeCell ref="K70:L72"/>
+    <mergeCell ref="N70:O72"/>
+    <mergeCell ref="P70:Q72"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="E70:G72"/>
+    <mergeCell ref="H70:I72"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="J81:M82"/>
+    <mergeCell ref="N81:Q82"/>
+    <mergeCell ref="B79:Q79"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="F80:I80"/>
+    <mergeCell ref="J80:M80"/>
+    <mergeCell ref="N80:Q80"/>
+    <mergeCell ref="H74:I76"/>
+    <mergeCell ref="E74:G76"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B81:E82"/>
+    <mergeCell ref="F81:I82"/>
+    <mergeCell ref="P74:Q76"/>
+    <mergeCell ref="N74:O76"/>
+    <mergeCell ref="K74:L76"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="K73:M73"/>
+    <mergeCell ref="K59:L61"/>
+    <mergeCell ref="N59:O61"/>
+    <mergeCell ref="P59:Q61"/>
+    <mergeCell ref="P63:Q65"/>
+    <mergeCell ref="N63:O65"/>
+    <mergeCell ref="K63:L65"/>
+    <mergeCell ref="H49:I51"/>
+    <mergeCell ref="E49:G51"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="B50:D50"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E59:G61"/>
+    <mergeCell ref="H59:I61"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="P49:Q51"/>
+    <mergeCell ref="N49:O51"/>
+    <mergeCell ref="K49:L51"/>
+    <mergeCell ref="H63:I65"/>
+    <mergeCell ref="E63:G65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E35:G37"/>
+    <mergeCell ref="H35:I37"/>
+    <mergeCell ref="K35:L37"/>
+    <mergeCell ref="N35:O37"/>
+    <mergeCell ref="P25:Q27"/>
+    <mergeCell ref="N25:O27"/>
+    <mergeCell ref="K25:L27"/>
+    <mergeCell ref="H25:I27"/>
+    <mergeCell ref="E25:G27"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="P35:Q37"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="P14:Q16"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E21:G23"/>
+    <mergeCell ref="H21:I23"/>
+    <mergeCell ref="K21:L23"/>
+    <mergeCell ref="N21:O23"/>
+    <mergeCell ref="P21:Q23"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="P9:Q9"/>
+    <mergeCell ref="P13:Q13"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="B20:D20"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="N4:Q4"/>
@@ -2916,160 +3064,6 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E10:G12"/>
     <mergeCell ref="E9:G9"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="P14:Q16"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E21:G23"/>
-    <mergeCell ref="H21:I23"/>
-    <mergeCell ref="K21:L23"/>
-    <mergeCell ref="N21:O23"/>
-    <mergeCell ref="P21:Q23"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E35:G37"/>
-    <mergeCell ref="H35:I37"/>
-    <mergeCell ref="K35:L37"/>
-    <mergeCell ref="N35:O37"/>
-    <mergeCell ref="P25:Q27"/>
-    <mergeCell ref="N25:O27"/>
-    <mergeCell ref="K25:L27"/>
-    <mergeCell ref="H25:I27"/>
-    <mergeCell ref="E25:G27"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="K59:L61"/>
-    <mergeCell ref="N59:O61"/>
-    <mergeCell ref="P59:Q61"/>
-    <mergeCell ref="P63:Q65"/>
-    <mergeCell ref="N63:O65"/>
-    <mergeCell ref="K63:L65"/>
-    <mergeCell ref="H49:I51"/>
-    <mergeCell ref="E49:G51"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B50:D50"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E59:G61"/>
-    <mergeCell ref="H59:I61"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="P49:Q51"/>
-    <mergeCell ref="N49:O51"/>
-    <mergeCell ref="K49:L51"/>
-    <mergeCell ref="H63:I65"/>
-    <mergeCell ref="E63:G65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="E70:G72"/>
-    <mergeCell ref="H70:I72"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="J81:M82"/>
-    <mergeCell ref="N81:Q82"/>
-    <mergeCell ref="B79:Q79"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="F80:I80"/>
-    <mergeCell ref="J80:M80"/>
-    <mergeCell ref="N80:Q80"/>
-    <mergeCell ref="H74:I76"/>
-    <mergeCell ref="E74:G76"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B81:E82"/>
-    <mergeCell ref="F81:I82"/>
-    <mergeCell ref="P74:Q76"/>
-    <mergeCell ref="N74:O76"/>
-    <mergeCell ref="K74:L76"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="K73:M73"/>
-    <mergeCell ref="N73:O73"/>
-    <mergeCell ref="P73:Q73"/>
-    <mergeCell ref="H69:J69"/>
-    <mergeCell ref="K69:M69"/>
-    <mergeCell ref="N69:O69"/>
-    <mergeCell ref="P69:Q69"/>
-    <mergeCell ref="K70:L72"/>
-    <mergeCell ref="N70:O72"/>
-    <mergeCell ref="P70:Q72"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E13:G13"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="K44:M44"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="P44:Q44"/>
-    <mergeCell ref="P48:Q48"/>
-    <mergeCell ref="N48:O48"/>
-    <mergeCell ref="K48:M48"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="K34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="P34:Q34"/>
-    <mergeCell ref="P38:Q38"/>
-    <mergeCell ref="K45:L47"/>
-    <mergeCell ref="N45:O47"/>
-    <mergeCell ref="P45:Q47"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="P9:Q9"/>
-    <mergeCell ref="P13:Q13"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="E48:G48"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E45:G47"/>
-    <mergeCell ref="H45:I47"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:J44"/>
-    <mergeCell ref="P35:Q37"/>
-    <mergeCell ref="P39:Q41"/>
-    <mergeCell ref="N39:O41"/>
-    <mergeCell ref="K39:L41"/>
-    <mergeCell ref="H39:I41"/>
-    <mergeCell ref="E39:G41"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="P24:Q24"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:O24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
@@ -3090,7 +3084,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3105,36 +3099,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="56" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="92" t="str">
-        <f>Bracket!L1 &amp; "; " &amp; Bracket!Q1</f>
-        <v xml:space="preserve">; </v>
-      </c>
-      <c r="C1" s="70"/>
+      <c r="A1" s="97" t="str">
+        <f>"Group# " &amp; Bracket!L1 &amp; "; Mat# " &amp; Bracket!Q1</f>
+        <v xml:space="preserve">Group# ; Mat# </v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="84"/>
       <c r="D1" s="52"/>
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
     </row>
-    <row r="2" spans="1:7" ht="39" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="57">
+    <row r="2" spans="1:7" ht="20" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="56">
         <f>Bracket!B3</f>
         <v>0</v>
       </c>
       <c r="B2" s="55"/>
-      <c r="C2" s="57">
+      <c r="C2" s="56">
         <f>Bracket!F3</f>
         <v>0</v>
       </c>
       <c r="D2" s="53"/>
-      <c r="E2" s="58">
+      <c r="E2" s="57">
         <f>Bracket!J3</f>
         <v>0</v>
       </c>
       <c r="F2" s="53"/>
-      <c r="G2" s="58">
+      <c r="G2" s="57">
         <f>Bracket!N3</f>
         <v>0</v>
       </c>
@@ -3164,7 +3156,7 @@
   </sheetData>
   <sheetProtection password="CFAF" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.1" right="0.1" top="0.25" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>